<commit_message>
Level 1 is finalized.
</commit_message>
<xml_diff>
--- a/02_Docs/DSS_Tables.xlsx
+++ b/02_Docs/DSS_Tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos_github\Enhanced_DSS\02_Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34658D84-A358-49F1-9FB8-37238364E40C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BEB5419-4009-4E19-BCD2-5FBFCF28DE40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{96F36749-A739-46FD-81F1-03E5F6C91E85}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2201" uniqueCount="845">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2201" uniqueCount="906">
   <si>
     <t>(Is there really a fire, and how certain are we?)</t>
   </si>
@@ -2072,9 +2072,6 @@
     <t>[{"label": "Very Low", "type": "gaussian", "mu": 6.0, "sigma": 7.199999999999999}, {"label": "Low", "type": "gaussian", "mu": 18.0, "sigma": 7.199999999999999}, {"label": "Medium", "type": "gaussian", "mu": 30.0, "sigma": 7.199999999999999}, {"label": "High", "type": "gaussian", "mu": 42.0, "sigma": 7.199999999999999}, {"label": "Very High", "type": "gaussian", "mu": 54.0, "sigma": 7.199999999999999}]</t>
   </si>
   <si>
-    <t>[{"label": "Very Low", "type": "gaussian", "mu": 2.0, "sigma": 2.4}, {"label": "Low", "type": "gaussian", "mu": 6.0, "sigma": 2.4}, {"label": "Medium", "type": "gaussian", "mu": 10.0, "sigma": 2.4}, {"label": "High", "type": "gaussian", "mu": 14.0, "sigma": 2.4}, {"label": "Very High", "type": "gaussian", "mu": 18.0, "sigma": 2.4}]</t>
-  </si>
-  <si>
     <t>[{"label": "Very Low", "type": "gaussian", "mu": 20.0, "sigma": 24.0}, {"label": "Low", "type": "gaussian", "mu": 60.0, "sigma": 24.0}, {"label": "Medium", "type": "gaussian", "mu": 100.0, "sigma": 24.0}, {"label": "High", "type": "gaussian", "mu": 140.0, "sigma": 24.0}, {"label": "Very High", "type": "gaussian", "mu": 180.0, "sigma": 24.0}]</t>
   </si>
   <si>
@@ -2447,27 +2444,9 @@
     <t>[{"label": "Very Low", "type": "trapezoid", "a": 0.0, "b": 0.0, "c": 0.2, "d": 0.35}, {"label": "Low", "type": "trapezoid", "a": 0.2, "b": 0.35, "c": 0.4, "d": 0.6}, {"label": "Medium", "type": "trapezoid", "a": 0.4, "b": 0.6, "c": 0.65, "d": 0.8}, {"label": "High", "type": "trapezoid", "a": 0.65, "b": 0.8, "c": 0.86, "d": 0.94}, {"label": "Very High", "type": "trapezoid", "a": 0.86, "b": 0.94, "c": 1.0, "d": 1.0}]</t>
   </si>
   <si>
-    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0.0, "b": 0.0, "c": 0.2, "d": 0.35}, {"label": "Low", "type": "trapezoid", "a": 0.2, "b": 0.35, "c": 0.45, "d": 0.6}, {"label": "Medium", "type": "trapezoid", "a": 0.45, "b": 0.6, "c": 0.7, "d": 0.82}, {"label": "High", "type": "trapezoid", "a": 0.7, "b": 0.82, "c": 0.9, "d": 0.96}, {"label": "Very High", "type": "trapezoid", "a": 0.9, "b": 0.96, "c": 1.0, "d": 1.0}]</t>
-  </si>
-  <si>
     <t>[{"label": "Very Low", "type": "trapezoid", "a": 0.0, "b": 0.0, "c": 0.3, "d": 0.5}, {"label": "Low", "type": "trapezoid", "a": 0.3, "b": 0.5, "c": 0.55, "d": 0.7}, {"label": "Medium", "type": "trapezoid", "a": 0.55, "b": 0.7, "c": 0.75, "d": 0.85}, {"label": "High", "type": "trapezoid", "a": 0.75, "b": 0.85, "c": 0.9, "d": 0.96}, {"label": "Very High", "type": "trapezoid", "a": 0.9, "b": 0.96, "c": 1.0, "d": 1.0}]</t>
   </si>
   <si>
-    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0.0, "b": 0.0, "c": 6.0, "d": 12.0}, {"label": "Low", "type": "trapezoid", "a": 2.999999999999999, "b": 9.0, "c": 21.0, "d": 27.0}, {"label": "Medium", "type": "trapezoid", "a": 18.0, "b": 24.0, "c": 36.0, "d": 42.0}, {"label": "High", "type": "trapezoid", "a": 33.0, "b": 39.0, "c": 51.0, "d": 57.0}, {"label": "Very High", "type": "trapezoid", "a": 48.0, "b": 54.0, "c": 60.0, "d": 60.0}]</t>
-  </si>
-  <si>
-    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0.0, "b": 0.0, "c": 50.0, "d": 100.0}, {"label": "Low", "type": "trapezoid", "a": 24.999999999999993, "b": 75.0, "c": 175.0, "d": 225.0}, {"label": "Medium", "type": "trapezoid", "a": 150.0, "b": 200.0, "c": 300.0, "d": 350.0}, {"label": "High", "type": "trapezoid", "a": 275.0, "b": 325.0, "c": 425.0, "d": 475.0}, {"label": "Very High", "type": "trapezoid", "a": 400.0, "b": 450.0, "c": 500.0, "d": 500.0}]</t>
-  </si>
-  <si>
-    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0.0, "b": 0.0, "c": 5.0, "d": 10.0}, {"label": "Low", "type": "trapezoid", "a": 2.4999999999999996, "b": 7.5, "c": 17.5, "d": 22.5}, {"label": "Medium", "type": "trapezoid", "a": 15.0, "b": 20.0, "c": 30.0, "d": 35.0}, {"label": "High", "type": "trapezoid", "a": 27.500000000000004, "b": 32.5, "c": 42.5, "d": 47.5}, {"label": "Very High", "type": "trapezoid", "a": 40.0, "b": 45.0, "c": 50.0, "d": 50.0}]</t>
-  </si>
-  <si>
-    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0.0, "b": 0.0, "c": 2000.0, "d": 4000.0}, {"label": "Low", "type": "trapezoid", "a": 999.9999999999998, "b": 3000.0, "c": 7000.0, "d": 9000.0}, {"label": "Medium", "type": "trapezoid", "a": 6000.0, "b": 8000.0, "c": 12000.0, "d": 14000.0}, {"label": "High", "type": "trapezoid", "a": 11000.0, "b": 13000.0, "c": 17000.0, "d": 19000.0}, {"label": "Very High", "type": "trapezoid", "a": 16000.0, "b": 18000.0, "c": 20000.0, "d": 20000.0}]</t>
-  </si>
-  <si>
-    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0.0, "b": 0.0, "c": 1000.0, "d": 2000.0}, {"label": "Low", "type": "trapezoid", "a": 499.9999999999999, "b": 1500.0, "c": 3500.0, "d": 4500.0}, {"label": "Medium", "type": "trapezoid", "a": 3000.0, "b": 4000.0, "c": 6000.0, "d": 7000.0}, {"label": "High", "type": "trapezoid", "a": 5500.0, "b": 6500.0, "c": 8500.0, "d": 9500.0}, {"label": "Very High", "type": "trapezoid", "a": 8000.0, "b": 9000.0, "c": 10000.0, "d": 10000.0}]</t>
-  </si>
-  <si>
     <t>[{"label": "Very Low", "type": "trapezoid", "a": 0.0, "b": 0.0, "c": 30.0, "d": 60.0}, {"label": "Low", "type": "trapezoid", "a": 14.999999999999996, "b": 45.0, "c": 105.0, "d": 135.0}, {"label": "Medium", "type": "trapezoid", "a": 90.0, "b": 120.0, "c": 180.0, "d": 210.0}, {"label": "High", "type": "trapezoid", "a": 165.0, "b": 195.0, "c": 255.0, "d": 285.0}, {"label": "Very High", "type": "trapezoid", "a": 240.0, "b": 270.0, "c": 300.0, "d": 300.0}]</t>
   </si>
   <si>
@@ -2492,21 +2471,9 @@
     <t>[{"label": "Very Low", "type": "trapezoid", "a": 0.0, "b": 0.0, "c": 10.0, "d": 20.0}, {"label": "Low", "type": "trapezoid", "a": 4.999999999999999, "b": 15.0, "c": 35.0, "d": 45.0}, {"label": "Medium", "type": "trapezoid", "a": 30.0, "b": 40.0, "c": 60.0, "d": 70.0}, {"label": "High", "type": "trapezoid", "a": 55.00000000000001, "b": 65.0, "c": 85.0, "d": 95.0}, {"label": "Very High", "type": "trapezoid", "a": 80.0, "b": 90.0, "c": 100.0, "d": 100.0}]</t>
   </si>
   <si>
-    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0.0, "b": 0.0, "c": 20.0, "d": 40.0}, {"label": "Low", "type": "trapezoid", "a": 9.999999999999998, "b": 30.0, "c": 70.0, "d": 90.0}, {"label": "Medium", "type": "trapezoid", "a": 60.0, "b": 80.0, "c": 120.0, "d": 140.0}, {"label": "High", "type": "trapezoid", "a": 110.00000000000001, "b": 130.0, "c": 170.0, "d": 190.0}, {"label": "Very High", "type": "trapezoid", "a": 160.0, "b": 180.0, "c": 200.0, "d": 200.0}]</t>
-  </si>
-  <si>
     <t>[{"label": "Very Low", "type": "trapezoid", "a": 0.0, "b": 0.0, "c": 5000.0, "d": 10000.0}, {"label": "Low", "type": "trapezoid", "a": 2499.9999999999995, "b": 7500.0, "c": 17500.0, "d": 22500.0}, {"label": "Medium", "type": "trapezoid", "a": 15000.0, "b": 20000.0, "c": 30000.0, "d": 35000.0}, {"label": "High", "type": "trapezoid", "a": 27500.000000000004, "b": 32500.0, "c": 42500.0, "d": 47500.0}, {"label": "Very High", "type": "trapezoid", "a": 40000.0, "b": 45000.0, "c": 50000.0, "d": 50000.0}]</t>
   </si>
   <si>
-    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0.0, "b": 0.0, "c": 2.4000000000000004, "d": 4.800000000000001}, {"label": "Low", "type": "trapezoid", "a": 1.1999999999999997, "b": 3.5999999999999996, "c": 8.399999999999999, "d": 10.8}, {"label": "Medium", "type": "trapezoid", "a": 7.199999999999999, "b": 9.600000000000001, "c": 14.399999999999999, "d": 16.799999999999997}, {"label": "High", "type": "trapezoid", "a": 13.200000000000001, "b": 15.600000000000001, "c": 20.4, "d": 22.799999999999997}, {"label": "Very High", "type": "trapezoid", "a": 19.200000000000003, "b": 21.6, "c": 24.0, "d": 24.0}]</t>
-  </si>
-  <si>
-    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0.0, "b": 0.0, "c": 500.0, "d": 1000.0}, {"label": "Low", "type": "trapezoid", "a": 249.99999999999994, "b": 750.0, "c": 1750.0, "d": 2250.0}, {"label": "Medium", "type": "trapezoid", "a": 1500.0, "b": 2000.0, "c": 3000.0, "d": 3500.0}, {"label": "High", "type": "trapezoid", "a": 2750.0, "b": 3250.0, "c": 4250.0, "d": 4750.0}, {"label": "Very High", "type": "trapezoid", "a": 4000.0, "b": 4500.0, "c": 5000.0, "d": 5000.0}]</t>
-  </si>
-  <si>
-    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0.0, "b": 0.0, "c": 100000.0, "d": 200000.0}, {"label": "Low", "type": "trapezoid", "a": 49999.999999999985, "b": 150000.0, "c": 350000.0, "d": 450000.0}, {"label": "Medium", "type": "trapezoid", "a": 300000.0, "b": 400000.0, "c": 600000.0, "d": 700000.0}, {"label": "High", "type": "trapezoid", "a": 550000.0, "b": 650000.0, "c": 850000.0, "d": 950000.0}, {"label": "Very High", "type": "trapezoid", "a": 800000.0, "b": 900000.0, "c": 1000000.0, "d": 1000000.0}]</t>
-  </si>
-  <si>
     <t>[{"label": "Very Low", "type": "trapezoid", "a": 0.0, "b": 0.0, "c": 500000.0, "d": 1000000.0}, {"label": "Low", "type": "trapezoid", "a": 249999.99999999994, "b": 750000.0, "c": 1750000.0, "d": 2250000.0}, {"label": "Medium", "type": "trapezoid", "a": 1500000.0, "b": 2000000.0, "c": 3000000.0, "d": 3500000.0}, {"label": "High", "type": "trapezoid", "a": 2750000.0, "b": 3250000.0, "c": 4250000.0, "d": 4750000.0}, {"label": "Very High", "type": "trapezoid", "a": 4000000.0, "b": 4500000.0, "c": 5000000.0, "d": 5000000.0}]</t>
   </si>
   <si>
@@ -2534,36 +2501,21 @@
     <t>[{"label": "Very Low", "type": "gaussian", "mu": 10.0, "sigma": 12.0}, {"label": "Low", "type": "gaussian", "mu": 30.0, "sigma": 12.0}, {"label": "Medium", "type": "gaussian", "mu": 50.0, "sigma": 12.0}, {"label": "High", "type": "gaussian", "mu": 70.0, "sigma": 12.0}, {"label": "Very High", "type": "gaussian", "mu": 90.0, "sigma": 12.0}]</t>
   </si>
   <si>
-    <t>[{"label": "Very Close", "type": "gaussian", "mu": 10.0, "sigma": 30.0}, {"label": "Close", "type": "gaussian", "mu": 40.0, "sigma": 30.0}, {"label": "Medium", "type": "gaussian", "mu": 90.0, "sigma": 30.0}, {"label": "Far", "type": "gaussian", "mu": 140.0, "sigma": 30.0}, {"label": "Very Far", "type": "gaussian", "mu": 180.0, "sigma": 30.0}]</t>
-  </si>
-  <si>
-    <t>[{"label": "N", "type": "circular_gaussian", "mu": 0.0, "sigma": 25.0}, {"label": "NE", "type": "circular_gaussian", "mu": 45.0, "sigma": 25.0}, {"label": "E", "type": "circular_gaussian", "mu": 90.0, "sigma": 25.0}, {"label": "SE", "type": "circular_gaussian", "mu": 135.0, "sigma": 25.0}, {"label": "S", "type": "circular_gaussian", "mu": 180.0, "sigma": 25.0}, {"label": "SW", "type": "circular_gaussian", "mu": 225.0, "sigma": 25.0}, {"label": "W", "type": "circular_gaussian", "mu": 270.0, "sigma": 25.0}, {"label": "NW", "type": "circular_gaussian", "mu": 315.0, "sigma": 25.0}]</t>
-  </si>
-  <si>
     <t>[{"label": "Very Low", "type": "trapezoid", "a": 0.0, "b": 0.0, "c": 0.2, "d": 0.4}, {"label": "Low", "type": "trapezoid", "a": 0.2, "b": 0.4, "c": 0.5, "d": 0.65}, {"label": "Medium", "type": "trapezoid", "a": 0.5, "b": 0.65, "c": 0.8, "d": 0.9}, {"label": "High", "type": "trapezoid", "a": 0.8, "b": 0.9, "c": 0.95, "d": 0.98}, {"label": "Very High", "type": "trapezoid", "a": 0.95, "b": 0.98, "c": 1.0, "d": 1.0}]</t>
   </si>
   <si>
     <t>Very Fast; Fast; Moderate; Slow; Very Slow</t>
   </si>
   <si>
-    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0.0, "b": 0.0, "c": 0.15, "d": 0.3}, {"label": "Low", "type": "trapezoid", "a": 0.15, "b": 0.3, "c": 0.3, "d": 0.45}, {"label": "Medium", "type": "trapezoid", "a": 0.3, "b": 0.45, "c": 0.8, "d": 0.85}, {"label": "High", "type": "trapezoid", "a": 0.8, "b": 0.85, "c": 0.95, "d": 0.98}, {"label": "Very High", "type": "trapezoid", "a": 0.95, "b": 0.98, "c": 1.0, "d": 1.0}]</t>
-  </si>
-  <si>
     <t>[{"label": "Very Fast", "type": "trapezoid", "a": 0.0, "b": 0.0, "c": 3.0, "d": 6.0}, {"label": "Fast", "type": "trapezoid", "a": 3.0, "b": 6.0, "c": 10.799999999999999, "d": 18.0}, {"label": "Moderate", "type": "trapezoid", "a": 10.799999999999999, "b": 18.0, "c": 27.0, "d": 36.0}, {"label": "Slow", "type": "trapezoid", "a": 27.0, "b": 36.0, "c": 45.0, "d": 52.8}, {"label": "Very Slow", "type": "trapezoid", "a": 45.0, "b": 52.8, "c": 60.0, "d": 60.0}]</t>
   </si>
   <si>
-    <t>[{"label": "Very Close", "type": "gaussian", "mu": 2.5, "sigma": 7.5}, {"label": "Close", "type": "gaussian", "mu": 10.0, "sigma": 7.5}, {"label": "Medium", "type": "gaussian", "mu": 22.5, "sigma": 7.5}, {"label": "Far", "type": "gaussian", "mu": 35.0, "sigma": 7.5}, {"label": "Very Far", "type": "gaussian", "mu": 45.0, "sigma": 7.5}]</t>
-  </si>
-  <si>
     <t>[{"label": "Very Fast", "type": "trapezoid", "a": 0.0, "b": 0.0, "c": 6.0, "d": 12.0}, {"label": "Fast", "type": "trapezoid", "a": 6.0, "b": 12.0, "c": 21.599999999999998, "d": 36.0}, {"label": "Moderate", "type": "trapezoid", "a": 21.599999999999998, "b": 36.0, "c": 54.0, "d": 72.0}, {"label": "Slow", "type": "trapezoid", "a": 54.0, "b": 72.0, "c": 90.0, "d": 105.6}, {"label": "Very Slow", "type": "trapezoid", "a": 90.0, "b": 105.6, "c": 120.0, "d": 120.0}]</t>
   </si>
   <si>
     <t>[{"label": "Very Fast", "type": "trapezoid", "a": 0.0, "b": 0.0, "c": 12.0, "d": 24.0}, {"label": "Fast", "type": "trapezoid", "a": 12.0, "b": 24.0, "c": 43.199999999999996, "d": 72.0}, {"label": "Moderate", "type": "trapezoid", "a": 43.199999999999996, "b": 72.0, "c": 108.0, "d": 144.0}, {"label": "Slow", "type": "trapezoid", "a": 108.0, "b": 144.0, "c": 180.0, "d": 211.2}, {"label": "Very Slow", "type": "trapezoid", "a": 180.0, "b": 211.2, "c": 240.0, "d": 240.0}]</t>
   </si>
   <si>
-    <t>[{'label': 'Very Low', 'type': 'trapezoid', 'a': 0, 'b': 0, 'c': 200, 'd': 500}, {'label': 'Low', 'type': 'trapezoid', 'a': 200, 'b': 500, 'c': 1200, 'd': 2500}, {'label': 'Medium', 'type': 'trapezoid', 'a': 1200, 'b': 2500, 'c': 4500, 'd': 6500}, {'label': 'High', 'type': 'trapezoid', 'a': 4500, 'b': 6500, 'c': 8000, 'd': 9000}, {'label': 'Very High', 'type': 'trapezoid', 'a': 8000, 'b': 9000, 'c': 10000, 'd': 10000}]</t>
-  </si>
-  <si>
     <t>Very Unstable; Unstable; Neutral; Stable; Very Stable</t>
   </si>
   <si>
@@ -2574,6 +2526,237 @@
   </si>
   <si>
     <t>[{"label": "Very Unstable", "type": "trapezoid", "a": 1.0, "b": 1.0, "c": 1.5, "d": 2.0}, {"label": "Unstable", "type": "trapezoid", "a": 1.25, "b": 1.75, "c": 2.75, "d": 3.25}, {"label": "Neutral", "type": "trapezoid", "a": 2.5, "b": 3.0, "c": 4.0, "d": 4.5}, {"label": "Stable", "type": "trapezoid", "a": 3.75, "b": 4.25, "c": 5.25, "d": 5.75}, {"label": "Very Stable", "type": "trapezoid", "a": 5.0, "b": 5.5, "c": 6.0, "d": 6.0}]</t>
+  </si>
+  <si>
+    <t>[{"label":"Very Low","type":"trapezoid","a":0.0,"b":0.0,"c":0.05,"d":0.15},{"label":"Low","type":"trapezoid","a":0.05,"b":0.15,"c":0.3,"d":0.45},{"label":"Medium","type":"trapezoid","a":0.3,"b":0.45,"c":0.6,"d":0.75},{"label":"High","type":"trapezoid","a":0.6,"b":0.75,"c":0.85,"d":0.95},{"label":"Very High","type":"trapezoid","a":0.85,"b":0.95,"c":1.0,"d":1.0}]</t>
+  </si>
+  <si>
+    <t>[{"label": "N", "type": "circular_gaussian", "mu": 0.000227, "sigma": 25.000227}, {"label": "NE", "type": "circular_gaussian", "mu": 45.000227, "sigma": 25.000227}, {"label": "E", "type": "circular_gaussian", "mu": 90.000227, "sigma": 25.000227}, {"label": "SE", "type": "circular_gaussian", "mu": 135.000227, "sigma": 25.000227}, {"label": "S", "type": "circular_gaussian", "mu": 180.000227, "sigma": 25.000227}, {"label": "SW", "type": "circular_gaussian", "mu": 225.000227, "sigma": 25.000227}, {"label": "W", "type": "circular_gaussian", "mu": 270.000227, "sigma": 25.000227}, {"label": "NW", "type": "circular_gaussian", "mu": 315.000227, "sigma": 25.000227}]</t>
+  </si>
+  <si>
+    <t>[{"label": "N", "type": "circular_gaussian", "mu": 0.000214, "sigma": 25.000214}, {"label": "NE", "type": "circular_gaussian", "mu": 45.000214, "sigma": 25.000214}, {"label": "E", "type": "circular_gaussian", "mu": 90.000214, "sigma": 25.000214}, {"label": "SE", "type": "circular_gaussian", "mu": 135.000214, "sigma": 25.000214}, {"label": "S", "type": "circular_gaussian", "mu": 180.000214, "sigma": 25.000214}, {"label": "SW", "type": "circular_gaussian", "mu": 225.000214, "sigma": 25.000214}, {"label": "W", "type": "circular_gaussian", "mu": 270.000214, "sigma": 25.000214}, {"label": "NW", "type": "circular_gaussian", "mu": 315.000214, "sigma": 25.000214}]</t>
+  </si>
+  <si>
+    <t>[{"label": "Very Low", "type": "gaussian", "mu": 2.000385, "sigma": 2.400385}, {"label": "Low", "type": "gaussian", "mu": 6.000385, "sigma": 2.400385}, {"label": "Medium", "type": "gaussian", "mu": 10.000385, "sigma": 2.400385}, {"label": "High", "type": "gaussian", "mu": 14.000385, "sigma": 2.400385}, {"label": "Very High", "type": "gaussian", "mu": 18.000385, "sigma": 2.400385}]</t>
+  </si>
+  <si>
+    <t>[{"label": "Very Low", "type": "gaussian", "mu": 2.000401, "sigma": 2.400401}, {"label": "Low", "type": "gaussian", "mu": 6.000401, "sigma": 2.400401}, {"label": "Medium", "type": "gaussian", "mu": 10.000401, "sigma": 2.400401}, {"label": "High", "type": "gaussian", "mu": 14.000401, "sigma": 2.400401}, {"label": "Very High", "type": "gaussian", "mu": 18.000401, "sigma": 2.400401}]</t>
+  </si>
+  <si>
+    <t>[{"label": "Very Close", "type": "gaussian", "mu": 2.500613, "sigma": 7.500613}, {"label": "Close", "type": "gaussian", "mu": 10.000613, "sigma": 7.500613}, {"label": "Medium", "type": "gaussian", "mu": 22.500613, "sigma": 7.500613}, {"label": "Far", "type": "gaussian", "mu": 35.000613, "sigma": 7.500613}, {"label": "Very Far", "type": "gaussian", "mu": 45.000613, "sigma": 7.500613}]</t>
+  </si>
+  <si>
+    <t>[{"label": "Very Close", "type": "gaussian", "mu": 2.500054, "sigma": 7.500054}, {"label": "Close", "type": "gaussian", "mu": 10.000054, "sigma": 7.500054}, {"label": "Medium", "type": "gaussian", "mu": 22.500054, "sigma": 7.500054}, {"label": "Far", "type": "gaussian", "mu": 35.000054, "sigma": 7.500054}, {"label": "Very Far", "type": "gaussian", "mu": 45.000054, "sigma": 7.500054}]</t>
+  </si>
+  <si>
+    <t>[{"label": "Very Close", "type": "gaussian", "mu": 2.500433, "sigma": 7.500433}, {"label": "Close", "type": "gaussian", "mu": 10.000433, "sigma": 7.500433}, {"label": "Medium", "type": "gaussian", "mu": 22.500433, "sigma": 7.500433}, {"label": "Far", "type": "gaussian", "mu": 35.000433, "sigma": 7.500433}, {"label": "Very Far", "type": "gaussian", "mu": 45.000433, "sigma": 7.500433}]</t>
+  </si>
+  <si>
+    <t>[{"label": "Very Close", "type": "gaussian", "mu": 10.000169, "sigma": 30.000169}, {"label": "Close", "type": "gaussian", "mu": 40.000169, "sigma": 30.000169}, {"label": "Medium", "type": "gaussian", "mu": 90.000169, "sigma": 30.000169}, {"label": "Far", "type": "gaussian", "mu": 140.000169, "sigma": 30.000169}, {"label": "Very Far", "type": "gaussian", "mu": 180.000169, "sigma": 30.000169}]</t>
+  </si>
+  <si>
+    <t>[{"label": "Very Close", "type": "gaussian", "mu": 10.000147, "sigma": 30.000147}, {"label": "Close", "type": "gaussian", "mu": 40.000147, "sigma": 30.000147}, {"label": "Medium", "type": "gaussian", "mu": 90.000147, "sigma": 30.000147}, {"label": "Far", "type": "gaussian", "mu": 140.000147, "sigma": 30.000147}, {"label": "Very Far", "type": "gaussian", "mu": 180.000147, "sigma": 30.000147}]</t>
+  </si>
+  <si>
+    <t>[ { "label": "Very Low", "type": "trapezoid", "a": 0, "b": 0, "c": 300, "d": 800 }, { "label": "Low", "type": "trapezoid", "a": 300, "b": 800, "c": 1500, "d": 2500 }, { "label": "Medium", "type": "trapezoid", "a": 1500, "b": 2500, "c": 4000, "d": 5500 }, { "label": "High", "type": "trapezoid", "a": 4000, "b": 5500, "c": 7500, "d": 9000 }, { "label": "Very High", "type": "trapezoid", "a": 7500, "b": 9000, "c": 10000, "d": 10000 } ]</t>
+  </si>
+  <si>
+    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0, "b": 0, "c": 0.097545, "d": 0.243045}, {"label": "Low", "type": "trapezoid", "a": 0.100545, "b": 0.250545, "c": 0.340045, "d": 0.485545}, {"label": "Medium", "type": "trapezoid", "a": 0.350545, "b": 0.500545, "c": 0.582545, "d": 0.728045}, {"label": "High", "type": "trapezoid", "a": 0.600545, "b": 0.750545, "c": 0.825045, "d": 0.922045}, {"label": "Very High", "type": "trapezoid", "a": 0.850545, "b": 0.950545, "c": 1, "d": 1}]</t>
+  </si>
+  <si>
+    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0, "b": 0, "c": 0.200641, "d": 0.350641}, {"label": "Low", "type": "trapezoid", "a": 0.200641, "b": 0.350641, "c": 0.450641, "d": 0.600641}, {"label": "Medium", "type": "trapezoid", "a": 0.450641, "b": 0.600641, "c": 0.750641, "d": 0.850641}, {"label": "High", "type": "trapezoid", "a": 0.750641, "b": 0.850641, "c": 0.950641, "d": 0.980641}, {"label": "Very High", "type": "trapezoid", "a": 0.950641, "b": 0.980641, "c": 1.0, "d": 1.0}]</t>
+  </si>
+  <si>
+    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0, "b": 0, "c": 0.097779, "d": 0.243279}, {"label": "Low", "type": "trapezoid", "a": 0.100779, "b": 0.250779, "c": 0.340279, "d": 0.485779}, {"label": "Medium", "type": "trapezoid", "a": 0.350779, "b": 0.500779, "c": 0.582779, "d": 0.728279}, {"label": "High", "type": "trapezoid", "a": 0.600779, "b": 0.750779, "c": 0.825279, "d": 0.922279}, {"label": "Very High", "type": "trapezoid", "a": 0.850779, "b": 0.950779, "c": 1, "d": 1}]</t>
+  </si>
+  <si>
+    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0, "b": 0, "c": 0.200822, "d": 0.350822}, {"label": "Low", "type": "trapezoid", "a": 0.200822, "b": 0.350822, "c": 0.450822, "d": 0.600822}, {"label": "Medium", "type": "trapezoid", "a": 0.450822, "b": 0.600822, "c": 0.750822, "d": 0.850822}, {"label": "High", "type": "trapezoid", "a": 0.750822, "b": 0.850822, "c": 0.950822, "d": 0.980822}, {"label": "Very High", "type": "trapezoid", "a": 0.950822, "b": 0.980822, "c": 1.0, "d": 1.0}]</t>
+  </si>
+  <si>
+    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0, "b": 0, "c": 2000.000005, "d": 4000.000005}, {"label": "Low", "type": "trapezoid", "a": 1000.000005, "b": 3000.000005, "c": 7000.000005, "d": 9000.000005}, {"label": "Medium", "type": "trapezoid", "a": 6000.000005, "b": 8000.000005, "c": 12000.000005, "d": 14000.000005}, {"label": "High", "type": "trapezoid", "a": 11000.000005, "b": 13000.000005, "c": 17000.000005, "d": 19000.000005}, {"label": "Very High", "type": "trapezoid", "a": 16000.000005, "b": 18000.000005, "c": 20000.0, "d": 20000.0}]</t>
+  </si>
+  <si>
+    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0, "b": 0, "c": 0.097064, "d": 0.242564}, {"label": "Low", "type": "trapezoid", "a": 0.100064, "b": 0.250064, "c": 0.339564, "d": 0.485064}, {"label": "Medium", "type": "trapezoid", "a": 0.350064, "b": 0.500064, "c": 0.582064, "d": 0.727564}, {"label": "High", "type": "trapezoid", "a": 0.600064, "b": 0.750064, "c": 0.824564, "d": 0.921564}, {"label": "Very High", "type": "trapezoid", "a": 0.850064, "b": 0.950064, "c": 1, "d": 1}]</t>
+  </si>
+  <si>
+    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0, "b": 0, "c": 0.097323, "d": 0.242823}, {"label": "Low", "type": "trapezoid", "a": 0.100323, "b": 0.250323, "c": 0.339823, "d": 0.485323}, {"label": "Medium", "type": "trapezoid", "a": 0.350323, "b": 0.500323, "c": 0.582323, "d": 0.727823}, {"label": "High", "type": "trapezoid", "a": 0.600323, "b": 0.750323, "c": 0.824823, "d": 0.921823}, {"label": "Very High", "type": "trapezoid", "a": 0.850323, "b": 0.950323, "c": 1, "d": 1}]</t>
+  </si>
+  <si>
+    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0, "b": 0, "c": 0.097085, "d": 0.242585}, {"label": "Low", "type": "trapezoid", "a": 0.100085, "b": 0.250085, "c": 0.339585, "d": 0.485085}, {"label": "Medium", "type": "trapezoid", "a": 0.350085, "b": 0.500085, "c": 0.582085, "d": 0.727585}, {"label": "High", "type": "trapezoid", "a": 0.600085, "b": 0.750085, "c": 0.824585, "d": 0.921585}, {"label": "Very High", "type": "trapezoid", "a": 0.850085, "b": 0.950085, "c": 1, "d": 1}]</t>
+  </si>
+  <si>
+    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0, "b": 0, "c": 0.145946, "d": 0.291446}, {"label": "Low", "type": "trapezoid", "a": 0.150446, "b": 0.300446, "c": 0.436946, "d": 0.582446}, {"label": "Medium", "type": "trapezoid", "a": 0.450446, "b": 0.600446, "c": 0.679446, "d": 0.824946}, {"label": "High", "type": "trapezoid", "a": 0.700446, "b": 0.850446, "c": 0.892846, "d": 0.941346}, {"label": "Very High", "type": "trapezoid", "a": 0.920446, "b": 0.970446, "c": 1, "d": 1}]</t>
+  </si>
+  <si>
+    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0, "b": 0, "c": 0.146152, "d": 0.291652}, {"label": "Low", "type": "trapezoid", "a": 0.150652, "b": 0.300652, "c": 0.437152, "d": 0.582652}, {"label": "Medium", "type": "trapezoid", "a": 0.450652, "b": 0.600652, "c": 0.679652, "d": 0.825152}, {"label": "High", "type": "trapezoid", "a": 0.700652, "b": 0.850652, "c": 0.893052, "d": 0.941552}, {"label": "Very High", "type": "trapezoid", "a": 0.920652, "b": 0.970652, "c": 1.0, "d": 1.0}]</t>
+  </si>
+  <si>
+    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0, "b": 0, "c": 0.146455, "d": 0.291955}, {"label": "Low", "type": "trapezoid", "a": 0.150955, "b": 0.300955, "c": 0.437455, "d": 0.582955}, {"label": "Medium", "type": "trapezoid", "a": 0.450955, "b": 0.600955, "c": 0.679955, "d": 0.825455}, {"label": "High", "type": "trapezoid", "a": 0.700955, "b": 0.850955, "c": 0.893355, "d": 0.941855}, {"label": "Very High", "type": "trapezoid", "a": 0.920955, "b": 0.970955, "c": 1, "d": 1}]</t>
+  </si>
+  <si>
+    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0, "b": 0, "c": 0.146014, "d": 0.291514}, {"label": "Low", "type": "trapezoid", "a": 0.150514, "b": 0.300514, "c": 0.437014, "d": 0.582514}, {"label": "Medium", "type": "trapezoid", "a": 0.450514, "b": 0.600514, "c": 0.679514, "d": 0.825014}, {"label": "High", "type": "trapezoid", "a": 0.700514, "b": 0.850514, "c": 0.892914, "d": 0.941414}, {"label": "Very High", "type": "trapezoid", "a": 0.920514, "b": 0.970514, "c": 1, "d": 1}]</t>
+  </si>
+  <si>
+    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0, "b": 0, "c": 6.00027, "d": 12.00027}, {"label": "Low", "type": "trapezoid", "a": 3.00027, "b": 9.00027, "c": 21.00027, "d": 27.00027}, {"label": "Medium", "type": "trapezoid", "a": 18.00027, "b": 24.00027, "c": 36.00027, "d": 42.00027}, {"label": "High", "type": "trapezoid", "a": 33.00027, "b": 39.00027, "c": 51.00027, "d": 57.00027}, {"label": "Very High", "type": "trapezoid", "a": 48.00027, "b": 54.00027, "c": 60.0, "d": 60.0}]</t>
+  </si>
+  <si>
+    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0, "b": 0, "c": 0.145958, "d": 0.291458}, {"label": "Low", "type": "trapezoid", "a": 0.150458, "b": 0.300458, "c": 0.436958, "d": 0.582458}, {"label": "Medium", "type": "trapezoid", "a": 0.450458, "b": 0.600458, "c": 0.679458, "d": 0.824958}, {"label": "High", "type": "trapezoid", "a": 0.700458, "b": 0.850458, "c": 0.892858, "d": 0.941358}, {"label": "Very High", "type": "trapezoid", "a": 0.920458, "b": 0.970458, "c": 1, "d": 1}]</t>
+  </si>
+  <si>
+    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0, "b": 0, "c": 0.146134, "d": 0.291634}, {"label": "Low", "type": "trapezoid", "a": 0.150634, "b": 0.300634, "c": 0.437134, "d": 0.582634}, {"label": "Medium", "type": "trapezoid", "a": 0.450634, "b": 0.600634, "c": 0.679634, "d": 0.825134}, {"label": "High", "type": "trapezoid", "a": 0.700634, "b": 0.850634, "c": 0.893034, "d": 0.941534}, {"label": "Very High", "type": "trapezoid", "a": 0.920634, "b": 0.970634, "c": 1, "d": 1}]</t>
+  </si>
+  <si>
+    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0, "b": 0, "c": 6.000419, "d": 12.000419}, {"label": "Low", "type": "trapezoid", "a": 3.000419, "b": 9.000419, "c": 21.000419, "d": 27.000419}, {"label": "Medium", "type": "trapezoid", "a": 18.000419, "b": 24.000419, "c": 36.000419, "d": 42.000419}, {"label": "High", "type": "trapezoid", "a": 33.000419, "b": 39.000419, "c": 51.000419, "d": 57.000419}, {"label": "Very High", "type": "trapezoid", "a": 48.000419, "b": 54.000419, "c": 60.0, "d": 60.0}]</t>
+  </si>
+  <si>
+    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0, "b": 0, "c": 0.097435, "d": 0.242935}, {"label": "Low", "type": "trapezoid", "a": 0.100435, "b": 0.250435, "c": 0.339935, "d": 0.485435}, {"label": "Medium", "type": "trapezoid", "a": 0.350435, "b": 0.500435, "c": 0.582435, "d": 0.727935}, {"label": "High", "type": "trapezoid", "a": 0.600435, "b": 0.750435, "c": 0.824935, "d": 0.921935}, {"label": "Very High", "type": "trapezoid", "a": 0.850435, "b": 0.950435, "c": 1.0, "d": 1.0}]</t>
+  </si>
+  <si>
+    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0, "b": 0, "c": 0.097269, "d": 0.242769}, {"label": "Low", "type": "trapezoid", "a": 0.100269, "b": 0.250269, "c": 0.339769, "d": 0.485269}, {"label": "Medium", "type": "trapezoid", "a": 0.350269, "b": 0.500269, "c": 0.582269, "d": 0.727769}, {"label": "High", "type": "trapezoid", "a": 0.600269, "b": 0.750269, "c": 0.824769, "d": 0.921769}, {"label": "Very High", "type": "trapezoid", "a": 0.850269, "b": 0.950269, "c": 1.0, "d": 1.0}]</t>
+  </si>
+  <si>
+    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0, "b": 0, "c": 0.097238, "d": 0.242738}, {"label": "Low", "type": "trapezoid", "a": 0.100238, "b": 0.250238, "c": 0.339738, "d": 0.485238}, {"label": "Medium", "type": "trapezoid", "a": 0.350238, "b": 0.500238, "c": 0.582238, "d": 0.727738}, {"label": "High", "type": "trapezoid", "a": 0.600238, "b": 0.750238, "c": 0.824738, "d": 0.921738}, {"label": "Very High", "type": "trapezoid", "a": 0.850238, "b": 0.950238, "c": 1, "d": 1}]</t>
+  </si>
+  <si>
+    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0, "b": 0, "c": 0.097256, "d": 0.242756}, {"label": "Low", "type": "trapezoid", "a": 0.100256, "b": 0.250256, "c": 0.339756, "d": 0.485256}, {"label": "Medium", "type": "trapezoid", "a": 0.350256, "b": 0.500256, "c": 0.582256, "d": 0.727756}, {"label": "High", "type": "trapezoid", "a": 0.600256, "b": 0.750256, "c": 0.824756, "d": 0.921756}, {"label": "Very High", "type": "trapezoid", "a": 0.850256, "b": 0.950256, "c": 1, "d": 1}]</t>
+  </si>
+  <si>
+    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0, "b": 0, "c": 0.145849, "d": 0.291349}, {"label": "Low", "type": "trapezoid", "a": 0.150349, "b": 0.300349, "c": 0.436849, "d": 0.582349}, {"label": "Medium", "type": "trapezoid", "a": 0.450349, "b": 0.600349, "c": 0.679349, "d": 0.824849}, {"label": "High", "type": "trapezoid", "a": 0.700349, "b": 0.850349, "c": 0.892749, "d": 0.941249}, {"label": "Very High", "type": "trapezoid", "a": 0.920349, "b": 0.970349, "c": 1, "d": 1}]</t>
+  </si>
+  <si>
+    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0, "b": 0, "c": 0.200219, "d": 0.350219}, {"label": "Low", "type": "trapezoid", "a": 0.200219, "b": 0.350219, "c": 0.450219, "d": 0.600219}, {"label": "Medium", "type": "trapezoid", "a": 0.450219, "b": 0.600219, "c": 0.750219, "d": 0.850219}, {"label": "High", "type": "trapezoid", "a": 0.750219, "b": 0.850219, "c": 0.950219, "d": 0.980219}, {"label": "Very High", "type": "trapezoid", "a": 0.950219, "b": 0.980219, "c": 1.0, "d": 1.0}]</t>
+  </si>
+  <si>
+    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0, "b": 0, "c": 0.200261, "d": 0.350261}, {"label": "Low", "type": "trapezoid", "a": 0.200261, "b": 0.350261, "c": 0.450261, "d": 0.600261}, {"label": "Medium", "type": "trapezoid", "a": 0.450261, "b": 0.600261, "c": 0.750261, "d": 0.850261}, {"label": "High", "type": "trapezoid", "a": 0.750261, "b": 0.850261, "c": 0.950261, "d": 0.980261}, {"label": "Very High", "type": "trapezoid", "a": 0.950261, "b": 0.980261, "c": 1.0, "d": 1.0}]</t>
+  </si>
+  <si>
+    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0, "b": 0, "c": 20.000042, "d": 40.000042}, {"label": "Low", "type": "trapezoid", "a": 10.000042, "b": 30.000042, "c": 70.000042, "d": 90.000042}, {"label": "Medium", "type": "trapezoid", "a": 60.000042, "b": 80.000042, "c": 120.000042, "d": 140.000042}, {"label": "High", "type": "trapezoid", "a": 110.000042, "b": 130.000042, "c": 170.000042, "d": 190.000042}, {"label": "Very High", "type": "trapezoid", "a": 160.000042, "b": 180.000042, "c": 200, "d": 200}]</t>
+  </si>
+  <si>
+    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0, "b": 0, "c": 0.097546, "d": 0.243046}, {"label": "Low", "type": "trapezoid", "a": 0.100546, "b": 0.250546, "c": 0.340046, "d": 0.485546}, {"label": "Medium", "type": "trapezoid", "a": 0.350546, "b": 0.500546, "c": 0.582546, "d": 0.728046}, {"label": "High", "type": "trapezoid", "a": 0.600546, "b": 0.750546, "c": 0.825046, "d": 0.922046}, {"label": "Very High", "type": "trapezoid", "a": 0.850546, "b": 0.950546, "c": 1, "d": 1}]</t>
+  </si>
+  <si>
+    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0, "b": 0, "c": 2000.000271, "d": 4000.000271}, {"label": "Low", "type": "trapezoid", "a": 1000.000271, "b": 3000.000271, "c": 7000.000271, "d": 9000.000271}, {"label": "Medium", "type": "trapezoid", "a": 6000.000271, "b": 8000.000271, "c": 12000.000271, "d": 14000.000271}, {"label": "High", "type": "trapezoid", "a": 11000.000271, "b": 13000.000271, "c": 17000.000271, "d": 19000.000271}, {"label": "Very High", "type": "trapezoid", "a": 16000.000271, "b": 18000.000271, "c": 20000, "d": 20000}]</t>
+  </si>
+  <si>
+    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0, "b": 0, "c": 2000.000896, "d": 4000.000896}, {"label": "Low", "type": "trapezoid", "a": 1000.000896, "b": 3000.000896, "c": 7000.000896, "d": 9000.000896}, {"label": "Medium", "type": "trapezoid", "a": 6000.000896, "b": 8000.000896, "c": 12000.000896, "d": 14000.000896}, {"label": "High", "type": "trapezoid", "a": 11000.000896, "b": 13000.000896, "c": 17000.000896, "d": 19000.000896}, {"label": "Very High", "type": "trapezoid", "a": 16000.000896, "b": 18000.000896, "c": 20000, "d": 20000}]</t>
+  </si>
+  <si>
+    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0, "b": 0, "c": 0.097478, "d": 0.242978}, {"label": "Low", "type": "trapezoid", "a": 0.100478, "b": 0.250478, "c": 0.339978, "d": 0.485478}, {"label": "Medium", "type": "trapezoid", "a": 0.350478, "b": 0.500478, "c": 0.582478, "d": 0.727978}, {"label": "High", "type": "trapezoid", "a": 0.600478, "b": 0.750478, "c": 0.824978, "d": 0.921978}, {"label": "Very High", "type": "trapezoid", "a": 0.850478, "b": 0.950478, "c": 1, "d": 1}]</t>
+  </si>
+  <si>
+    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0, "b": 0, "c": 0.097038, "d": 0.242538}, {"label": "Low", "type": "trapezoid", "a": 0.100038, "b": 0.250038, "c": 0.339538, "d": 0.485038}, {"label": "Medium", "type": "trapezoid", "a": 0.350038, "b": 0.500038, "c": 0.582038, "d": 0.727538}, {"label": "High", "type": "trapezoid", "a": 0.600038, "b": 0.750038, "c": 0.824538, "d": 0.921538}, {"label": "Very High", "type": "trapezoid", "a": 0.850038, "b": 0.950038, "c": 1, "d": 1}]</t>
+  </si>
+  <si>
+    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0, "b": 0, "c": 0.097827, "d": 0.243327}, {"label": "Low", "type": "trapezoid", "a": 0.100827, "b": 0.250827, "c": 0.340327, "d": 0.485827}, {"label": "Medium", "type": "trapezoid", "a": 0.350827, "b": 0.500827, "c": 0.582827, "d": 0.728327}, {"label": "High", "type": "trapezoid", "a": 0.600827, "b": 0.750827, "c": 0.825327, "d": 0.922327}, {"label": "Very High", "type": "trapezoid", "a": 0.850827, "b": 0.950827, "c": 1, "d": 1}]</t>
+  </si>
+  <si>
+    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0, "b": 0, "c": 0.09762, "d": 0.24312}, {"label": "Low", "type": "trapezoid", "a": 0.10062, "b": 0.25062, "c": 0.34012, "d": 0.48562}, {"label": "Medium", "type": "trapezoid", "a": 0.35062, "b": 0.50062, "c": 0.58262, "d": 0.72812}, {"label": "High", "type": "trapezoid", "a": 0.60062, "b": 0.75062, "c": 0.82512, "d": 0.92212}, {"label": "Very High", "type": "trapezoid", "a": 0.85062, "b": 0.95062, "c": 1, "d": 1}]</t>
+  </si>
+  <si>
+    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0, "b": 0, "c": 0.097045, "d": 0.242545}, {"label": "Low", "type": "trapezoid", "a": 0.100045, "b": 0.250045, "c": 0.339545, "d": 0.485045}, {"label": "Medium", "type": "trapezoid", "a": 0.350045, "b": 0.500045, "c": 0.582045, "d": 0.727545}, {"label": "High", "type": "trapezoid", "a": 0.600045, "b": 0.750045, "c": 0.824545, "d": 0.921545}, {"label": "Very High", "type": "trapezoid", "a": 0.850045, "b": 0.950045, "c": 1, "d": 1}]</t>
+  </si>
+  <si>
+    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0, "b": 0, "c": 0.097609, "d": 0.243109}, {"label": "Low", "type": "trapezoid", "a": 0.100609, "b": 0.250609, "c": 0.340109, "d": 0.485609}, {"label": "Medium", "type": "trapezoid", "a": 0.350609, "b": 0.500609, "c": 0.582609, "d": 0.728109}, {"label": "High", "type": "trapezoid", "a": 0.600609, "b": 0.750609, "c": 0.825109, "d": 0.922109}, {"label": "Very High", "type": "trapezoid", "a": 0.850609, "b": 0.950609, "c": 1, "d": 1}]</t>
+  </si>
+  <si>
+    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0, "b": 0, "c": 0.097141, "d": 0.242641}, {"label": "Low", "type": "trapezoid", "a": 0.100141, "b": 0.250141, "c": 0.339641, "d": 0.485141}, {"label": "Medium", "type": "trapezoid", "a": 0.350141, "b": 0.500141, "c": 0.582141, "d": 0.727641}, {"label": "High", "type": "trapezoid", "a": 0.600141, "b": 0.750141, "c": 0.824641, "d": 0.921641}, {"label": "Very High", "type": "trapezoid", "a": 0.850141, "b": 0.950141, "c": 1, "d": 1}]</t>
+  </si>
+  <si>
+    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0, "b": 0, "c": 1000.000431, "d": 2000.000431}, {"label": "Low", "type": "trapezoid", "a": 500.000431, "b": 1500.000431, "c": 3500.000431, "d": 4500.000431}, {"label": "Medium", "type": "trapezoid", "a": 3000.000431, "b": 4000.000431, "c": 6000.000431, "d": 7000.000431}, {"label": "High", "type": "trapezoid", "a": 5500.000431, "b": 6500.000431, "c": 8500.000431, "d": 9500.000431}, {"label": "Very High", "type": "trapezoid", "a": 8000.000431, "b": 9000.000431, "c": 10000, "d": 10000}]</t>
+  </si>
+  <si>
+    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0, "b": 0, "c": 20.000349, "d": 40.000349}, {"label": "Low", "type": "trapezoid", "a": 10.000349, "b": 30.000349, "c": 70.000349, "d": 90.000349}, {"label": "Medium", "type": "trapezoid", "a": 60.000349, "b": 80.000349, "c": 120.000349, "d": 140.000349}, {"label": "High", "type": "trapezoid", "a": 110.000349, "b": 130.000349, "c": 170.000349, "d": 190.000349}, {"label": "Very High", "type": "trapezoid", "a": 160.000349, "b": 180.000349, "c": 200, "d": 200}]</t>
+  </si>
+  <si>
+    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0, "b": 0, "c": 2.400721, "d": 4.800721}, {"label": "Low", "type": "trapezoid", "a": 1.200721, "b": 3.600721, "c": 8.400721, "d": 10.800721}, {"label": "Medium", "type": "trapezoid", "a": 7.200721, "b": 9.600721, "c": 14.400721, "d": 16.800721}, {"label": "High", "type": "trapezoid", "a": 13.200721, "b": 15.600721, "c": 20.400721, "d": 22.800721}, {"label": "Very High", "type": "trapezoid", "a": 19.200721, "b": 21.600721, "c": 24, "d": 24}]</t>
+  </si>
+  <si>
+    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0, "b": 0, "c": 20.000713, "d": 40.000713}, {"label": "Low", "type": "trapezoid", "a": 10.000713, "b": 30.000713, "c": 70.000713, "d": 90.000713}, {"label": "Medium", "type": "trapezoid", "a": 60.000713, "b": 80.000713, "c": 120.000713, "d": 140.000713}, {"label": "High", "type": "trapezoid", "a": 110.000713, "b": 130.000713, "c": 170.000713, "d": 190.000713}, {"label": "Very High", "type": "trapezoid", "a": 160.000713, "b": 180.000713, "c": 200, "d": 200}]</t>
+  </si>
+  <si>
+    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0, "b": 0, "c": 2000.000872, "d": 4000.000872}, {"label": "Low", "type": "trapezoid", "a": 1000.000872, "b": 3000.000872, "c": 7000.000872, "d": 9000.000872}, {"label": "Medium", "type": "trapezoid", "a": 6000.000872, "b": 8000.000872, "c": 12000.000872, "d": 14000.000872}, {"label": "High", "type": "trapezoid", "a": 11000.000872, "b": 13000.000872, "c": 17000.000872, "d": 19000.000872}, {"label": "Very High", "type": "trapezoid", "a": 16000.000872, "b": 18000.000872, "c": 20000, "d": 20000}]</t>
+  </si>
+  <si>
+    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0, "b": 0, "c": 500.000694, "d": 1000.000694}, {"label": "Low", "type": "trapezoid", "a": 250.000694, "b": 750.000694, "c": 1750.000694, "d": 2250.000694}, {"label": "Medium", "type": "trapezoid", "a": 1500.000694, "b": 2000.000694, "c": 3000.000694, "d": 3500.000694}, {"label": "High", "type": "trapezoid", "a": 2750.000694, "b": 3250.000694, "c": 4250.000694, "d": 4750.000694}, {"label": "Very High", "type": "trapezoid", "a": 4000.000694, "b": 4500.000694, "c": 5000, "d": 5000}]</t>
+  </si>
+  <si>
+    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0, "b": 0, "c": 0.097942, "d": 0.243442}, {"label": "Low", "type": "trapezoid", "a": 0.100942, "b": 0.250942, "c": 0.340442, "d": 0.485942}, {"label": "Medium", "type": "trapezoid", "a": 0.350942, "b": 0.500942, "c": 0.582942, "d": 0.728442}, {"label": "High", "type": "trapezoid", "a": 0.600942, "b": 0.750942, "c": 0.825442, "d": 0.922442}, {"label": "Very High", "type": "trapezoid", "a": 0.850942, "b": 0.950942, "c": 1, "d": 1}]</t>
+  </si>
+  <si>
+    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0, "b": 0, "c": 5.000052, "d": 10.000052}, {"label": "Low", "type": "trapezoid", "a": 2.500052, "b": 7.500052, "c": 17.500052, "d": 22.500052}, {"label": "Medium", "type": "trapezoid", "a": 15.000052, "b": 20.000052, "c": 30.000052, "d": 35.000052}, {"label": "High", "type": "trapezoid", "a": 27.500052, "b": 32.500052, "c": 42.500052, "d": 47.500052}, {"label": "Very High", "type": "trapezoid", "a": 40.000052, "b": 45.000052, "c": 50, "d": 50}]</t>
+  </si>
+  <si>
+    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0, "b": 0, "c": 5.000372, "d": 10.000372}, {"label": "Low", "type": "trapezoid", "a": 2.500372, "b": 7.500372, "c": 17.500372, "d": 22.500372}, {"label": "Medium", "type": "trapezoid", "a": 15.000372, "b": 20.000372, "c": 30.000372, "d": 35.000372}, {"label": "High", "type": "trapezoid", "a": 27.500372, "b": 32.500372, "c": 42.500372, "d": 47.500372}, {"label": "Very High", "type": "trapezoid", "a": 40.000372, "b": 45.000372, "c": 50, "d": 50}]</t>
+  </si>
+  <si>
+    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0, "b": 0, "c": 0.09765, "d": 0.24315}, {"label": "Low", "type": "trapezoid", "a": 0.10065, "b": 0.25065, "c": 0.34015, "d": 0.48565}, {"label": "Medium", "type": "trapezoid", "a": 0.35065, "b": 0.50065, "c": 0.58265, "d": 0.72815}, {"label": "High", "type": "trapezoid", "a": 0.60065, "b": 0.75065, "c": 0.82515, "d": 0.92215}, {"label": "Very High", "type": "trapezoid", "a": 0.85065, "b": 0.95065, "c": 1, "d": 1}]</t>
+  </si>
+  <si>
+    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0, "b": 0, "c": 5.00096, "d": 10.00096}, {"label": "Low", "type": "trapezoid", "a": 2.50096, "b": 7.50096, "c": 17.50096, "d": 22.50096}, {"label": "Medium", "type": "trapezoid", "a": 15.00096, "b": 20.00096, "c": 30.00096, "d": 35.00096}, {"label": "High", "type": "trapezoid", "a": 27.50096, "b": 32.50096, "c": 42.50096, "d": 47.50096}, {"label": "Very High", "type": "trapezoid", "a": 40.00096, "b": 45.00096, "c": 50, "d": 50}]</t>
+  </si>
+  <si>
+    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0, "b": 0, "c": 2000.000934, "d": 4000.000934}, {"label": "Low", "type": "trapezoid", "a": 1000.000934, "b": 3000.000934, "c": 7000.000934, "d": 9000.000934}, {"label": "Medium", "type": "trapezoid", "a": 6000.000934, "b": 8000.000934, "c": 12000.000934, "d": 14000.000934}, {"label": "High", "type": "trapezoid", "a": 11000.000934, "b": 13000.000934, "c": 17000.000934, "d": 19000.000934}, {"label": "Very High", "type": "trapezoid", "a": 16000.000934, "b": 18000.000934, "c": 20000, "d": 20000}]</t>
+  </si>
+  <si>
+    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0, "b": 0, "c": 1000.000352, "d": 2000.000352}, {"label": "Low", "type": "trapezoid", "a": 500.000352, "b": 1500.000352, "c": 3500.000352, "d": 4500.000352}, {"label": "Medium", "type": "trapezoid", "a": 3000.000352, "b": 4000.000352, "c": 6000.000352, "d": 7000.000352}, {"label": "High", "type": "trapezoid", "a": 5500.000352, "b": 6500.000352, "c": 8500.000352, "d": 9500.000352}, {"label": "Very High", "type": "trapezoid", "a": 8000.000352, "b": 9000.000352, "c": 10000, "d": 10000}]</t>
+  </si>
+  <si>
+    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0, "b": 0, "c": 20.000768, "d": 40.000768}, {"label": "Low", "type": "trapezoid", "a": 10.000768, "b": 30.000768, "c": 70.000768, "d": 90.000768}, {"label": "Medium", "type": "trapezoid", "a": 60.000768, "b": 80.000768, "c": 120.000768, "d": 140.000768}, {"label": "High", "type": "trapezoid", "a": 110.000768, "b": 130.000768, "c": 170.000768, "d": 190.000768}, {"label": "Very High", "type": "trapezoid", "a": 160.000768, "b": 180.000768, "c": 200, "d": 200}]</t>
+  </si>
+  <si>
+    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0, "b": 0, "c": 0.145599, "d": 0.291099}, {"label": "Low", "type": "trapezoid", "a": 0.150099, "b": 0.300099, "c": 0.388099, "d": 0.533599}, {"label": "Medium", "type": "trapezoid", "a": 0.400099, "b": 0.550099, "c": 0.630599, "d": 0.727599}, {"label": "High", "type": "trapezoid", "a": 0.650099, "b": 0.750099, "c": 0.873099, "d": 0.940999}, {"label": "Very High", "type": "trapezoid", "a": 0.900099, "b": 0.970099, "c": 1, "d": 1}]</t>
+  </si>
+  <si>
+    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0, "b": 0, "c": 100000.000703, "d": 200000.000703}, {"label": "Low", "type": "trapezoid", "a": 50000.000703, "b": 150000.000703, "c": 350000.000703, "d": 450000.000703}, {"label": "Medium", "type": "trapezoid", "a": 300000.000703, "b": 400000.000703, "c": 600000.000703, "d": 700000.000703}, {"label": "High", "type": "trapezoid", "a": 550000.000703, "b": 650000.000703, "c": 850000.000703, "d": 950000.000703}, {"label": "Very High", "type": "trapezoid", "a": 800000.000703, "b": 900000.000703, "c": 1000000, "d": 1000000}]</t>
+  </si>
+  <si>
+    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0, "b": 0, "c": 100000.000707, "d": 200000.000707}, {"label": "Low", "type": "trapezoid", "a": 50000.000707, "b": 150000.000707, "c": 350000.000707, "d": 450000.000707}, {"label": "Medium", "type": "trapezoid", "a": 300000.000707, "b": 400000.000707, "c": 600000.000707, "d": 700000.000707}, {"label": "High", "type": "trapezoid", "a": 550000.000707, "b": 650000.000707, "c": 850000.000707, "d": 950000.000707}, {"label": "Very High", "type": "trapezoid", "a": 800000.000707, "b": 900000.000707, "c": 1000000, "d": 1000000}]</t>
+  </si>
+  <si>
+    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0, "b": 0, "c": 0.097587, "d": 0.243087}, {"label": "Low", "type": "trapezoid", "a": 0.100587, "b": 0.250587, "c": 0.340087, "d": 0.485587}, {"label": "Medium", "type": "trapezoid", "a": 0.350587, "b": 0.500587, "c": 0.582587, "d": 0.728087}, {"label": "High", "type": "trapezoid", "a": 0.600587, "b": 0.750587, "c": 0.825087, "d": 0.922087}, {"label": "Very High", "type": "trapezoid", "a": 0.850587, "b": 0.950587, "c": 1, "d": 1}]</t>
+  </si>
+  <si>
+    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0, "b": 0, "c": 100000.000112, "d": 200000.000112}, {"label": "Low", "type": "trapezoid", "a": 50000.000112, "b": 150000.000112, "c": 350000.000112, "d": 450000.000112}, {"label": "Medium", "type": "trapezoid", "a": 300000.000112, "b": 400000.000112, "c": 600000.000112, "d": 700000.000112}, {"label": "High", "type": "trapezoid", "a": 550000.000112, "b": 650000.000112, "c": 850000.000112, "d": 950000.000112}, {"label": "Very High", "type": "trapezoid", "a": 800000.000112, "b": 900000.000112, "c": 1000000, "d": 1000000}]</t>
+  </si>
+  <si>
+    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0, "b": 0, "c": 500.000079, "d": 1000.000079}, {"label": "Low", "type": "trapezoid", "a": 250.000079, "b": 750.000079, "c": 1750.000079, "d": 2250.000079}, {"label": "Medium", "type": "trapezoid", "a": 1500.000079, "b": 2000.000079, "c": 3000.000079, "d": 3500.000079}, {"label": "High", "type": "trapezoid", "a": 2750.000079, "b": 3250.000079, "c": 4250.000079, "d": 4750.000079}, {"label": "Very High", "type": "trapezoid", "a": 4000.000079, "b": 4500.000079, "c": 5000, "d": 5000}]</t>
+  </si>
+  <si>
+    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0, "b": 0, "c": 50.000349, "d": 100.000349}, {"label": "Low", "type": "trapezoid", "a": 25.000349, "b": 75.000349, "c": 175.000349, "d": 225.000349}, {"label": "Medium", "type": "trapezoid", "a": 150.000349, "b": 200.000349, "c": 300.000349, "d": 350.000349}, {"label": "High", "type": "trapezoid", "a": 275.000349, "b": 325.000349, "c": 425.000349, "d": 475.000349}, {"label": "Very High", "type": "trapezoid", "a": 400.000349, "b": 450.000349, "c": 500, "d": 500}]</t>
+  </si>
+  <si>
+    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0, "b": 0, "c": 100000.000713, "d": 200000.000713}, {"label": "Low", "type": "trapezoid", "a": 50000.000713, "b": 150000.000713, "c": 350000.000713, "d": 450000.000713}, {"label": "Medium", "type": "trapezoid", "a": 300000.000713, "b": 400000.000713, "c": 600000.000713, "d": 700000.000713}, {"label": "High", "type": "trapezoid", "a": 550000.000713, "b": 650000.000713, "c": 850000.000713, "d": 950000.000713}, {"label": "Very High", "type": "trapezoid", "a": 800000.000713, "b": 900000.000713, "c": 1000000, "d": 1000000}]</t>
+  </si>
+  <si>
+    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0, "b": 0, "c": 20.00021, "d": 40.00021}, {"label": "Low", "type": "trapezoid", "a": 10.00021, "b": 30.00021, "c": 70.00021, "d": 90.00021}, {"label": "Medium", "type": "trapezoid", "a": 60.00021, "b": 80.00021, "c": 120.00021, "d": 140.00021}, {"label": "High", "type": "trapezoid", "a": 110.00021, "b": 130.00021, "c": 170.00021, "d": 190.00021}, {"label": "Very High", "type": "trapezoid", "a": 160.00021, "b": 180.00021, "c": 200, "d": 200}]</t>
+  </si>
+  <si>
+    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0, "b": 0, "c": 50.000914, "d": 100.000914}, {"label": "Low", "type": "trapezoid", "a": 25.000914, "b": 75.000914, "c": 175.000914, "d": 225.000914}, {"label": "Medium", "type": "trapezoid", "a": 150.000914, "b": 200.000914, "c": 300.000914, "d": 350.000914}, {"label": "High", "type": "trapezoid", "a": 275.000914, "b": 325.000914, "c": 425.000914, "d": 475.000914}, {"label": "Very High", "type": "trapezoid", "a": 400.000914, "b": 450.000914, "c": 500, "d": 500}]</t>
+  </si>
+  <si>
+    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0, "b": 0, "c": 0.145812, "d": 0.291312}, {"label": "Low", "type": "trapezoid", "a": 0.150312, "b": 0.300312, "c": 0.388312, "d": 0.533812}, {"label": "Medium", "type": "trapezoid", "a": 0.400312, "b": 0.550312, "c": 0.630812, "d": 0.727812}, {"label": "High", "type": "trapezoid", "a": 0.650312, "b": 0.750312, "c": 0.873312, "d": 0.941212}, {"label": "Very High", "type": "trapezoid", "a": 0.900312, "b": 0.970312, "c": 1, "d": 1}]</t>
+  </si>
+  <si>
+    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0, "b": 0, "c": 0.20065, "d": 0.35065}, {"label": "Low", "type": "trapezoid", "a": 0.20065, "b": 0.35065, "c": 0.45065, "d": 0.60065}, {"label": "Medium", "type": "trapezoid", "a": 0.45065, "b": 0.60065, "c": 0.75065, "d": 0.85065}, {"label": "High", "type": "trapezoid", "a": 0.75065, "b": 0.85065, "c": 0.95065, "d": 0.98065}, {"label": "Very High", "type": "trapezoid", "a": 0.95065, "b": 0.98065, "c": 1.0, "d": 1.0}]</t>
+  </si>
+  <si>
+    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0, "b": 0, "c": 0.097188, "d": 0.242688}, {"label": "Low", "type": "trapezoid", "a": 0.100188, "b": 0.250188, "c": 0.339688, "d": 0.485188}, {"label": "Medium", "type": "trapezoid", "a": 0.350188, "b": 0.500188, "c": 0.582188, "d": 0.727688}, {"label": "High", "type": "trapezoid", "a": 0.600188, "b": 0.750188, "c": 0.824688, "d": 0.921688}, {"label": "Very High", "type": "trapezoid", "a": 0.850188, "b": 0.950188, "c": 1, "d": 1}]</t>
+  </si>
+  <si>
+    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0, "b": 0, "c": 500.00038, "d": 1000.00038}, {"label": "Low", "type": "trapezoid", "a": 250.00038, "b": 750.00038, "c": 1750.00038, "d": 2250.00038}, {"label": "Medium", "type": "trapezoid", "a": 1500.00038, "b": 2000.00038, "c": 3000.00038, "d": 3500.00038}, {"label": "High", "type": "trapezoid", "a": 2750.00038, "b": 3250.00038, "c": 4250.00038, "d": 4750.00038}, {"label": "Very High", "type": "trapezoid", "a": 4000.00038, "b": 4500.00038, "c": 5000, "d": 5000}]</t>
+  </si>
+  <si>
+    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0, "b": 0, "c": 0.097411, "d": 0.242911}, {"label": "Low", "type": "trapezoid", "a": 0.100411, "b": 0.250411, "c": 0.339911, "d": 0.485411}, {"label": "Medium", "type": "trapezoid", "a": 0.350411, "b": 0.500411, "c": 0.582411, "d": 0.727911}, {"label": "High", "type": "trapezoid", "a": 0.600411, "b": 0.750411, "c": 0.824911, "d": 0.921911}, {"label": "Very High", "type": "trapezoid", "a": 0.850411, "b": 0.950411, "c": 1, "d": 1}]</t>
+  </si>
+  <si>
+    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0, "b": 0, "c": 1000.000394, "d": 2000.000394}, {"label": "Low", "type": "trapezoid", "a": 500.000394, "b": 1500.000394, "c": 3500.000394, "d": 4500.000394}, {"label": "Medium", "type": "trapezoid", "a": 3000.000394, "b": 4000.000394, "c": 6000.000394, "d": 7000.000394}, {"label": "High", "type": "trapezoid", "a": 5500.000394, "b": 6500.000394, "c": 8500.000394, "d": 9500.000394}, {"label": "Very High", "type": "trapezoid", "a": 8000.000394, "b": 9000.000394, "c": 10000, "d": 10000}]</t>
+  </si>
+  <si>
+    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0, "b": 0, "c": 2.400267, "d": 4.800267}, {"label": "Low", "type": "trapezoid", "a": 1.200267, "b": 3.600267, "c": 8.400267, "d": 10.800267}, {"label": "Medium", "type": "trapezoid", "a": 7.200267, "b": 9.600267, "c": 14.400267, "d": 16.800267}, {"label": "High", "type": "trapezoid", "a": 13.200267, "b": 15.600267, "c": 20.400267, "d": 22.800267}, {"label": "Very High", "type": "trapezoid", "a": 19.200267, "b": 21.600267, "c": 24, "d": 24}]</t>
+  </si>
+  <si>
+    <t>[{"label": "Very Low", "type": "trapezoid", "a": 0, "b": 0, "c": 20.000055, "d": 40.000055}, {"label": "Low", "type": "trapezoid", "a": 10.000055, "b": 30.000055, "c": 70.000055, "d": 90.000055}, {"label": "Medium", "type": "trapezoid", "a": 60.000055, "b": 80.000055, "c": 120.000055, "d": 140.000055}, {"label": "High", "type": "trapezoid", "a": 110.000055, "b": 130.000055, "c": 170.000055, "d": 190.000055}, {"label": "Very High", "type": "trapezoid", "a": 160.000055, "b": 180.000055, "c": 200, "d": 200}]</t>
   </si>
 </sst>
 </file>
@@ -2693,43 +2876,40 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="26">
+  <dxfs count="25">
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2832,7 +3012,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0D0EB180-066E-49D5-BE38-124E6B5EFC6A}" name="Table1" displayName="Table1" ref="A1:B1048576" totalsRowShown="0" headerRowBorderDxfId="25" tableBorderDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0D0EB180-066E-49D5-BE38-124E6B5EFC6A}" name="Table1" displayName="Table1" ref="A1:B1048576" totalsRowShown="0" headerRowBorderDxfId="24" tableBorderDxfId="23">
   <autoFilter ref="A1:B1048576" xr:uid="{0D0EB180-066E-49D5-BE38-124E6B5EFC6A}"/>
   <tableColumns count="2">
     <tableColumn id="2" xr3:uid="{10FE7A06-DF2D-4D9F-A91B-67B5EC52B56D}" name="Question Category"/>
@@ -2843,25 +3023,25 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{14A13433-3602-4EAD-8991-345F6C09DA18}" name="Table4" displayName="Table4" ref="A1:I118" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{14A13433-3602-4EAD-8991-345F6C09DA18}" name="Table4" displayName="Table4" ref="A1:I118" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
   <autoFilter ref="A1:I118" xr:uid="{14A13433-3602-4EAD-8991-345F6C09DA18}"/>
   <tableColumns count="9">
-    <tableColumn id="13" xr3:uid="{8D7C28EE-960A-49A1-9FFC-CF5BAFA26C18}" name="Contributes To Question Types" dataDxfId="21"/>
-    <tableColumn id="1" xr3:uid="{AD6576F3-D2B1-477D-A460-9D7D8F000211}" name="Level1 Category" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{0C27C753-AF92-4769-9D92-64781AA12529}" name="Data Class" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{0347D29C-0658-4470-8597-C2BEB668EA32}" name="Observable Quantity" dataDxfId="18"/>
-    <tableColumn id="8" xr3:uid="{2418DCB6-00EA-4B5D-955A-FC9E0439D4FC}" name="Spatial Resolution" dataDxfId="17"/>
-    <tableColumn id="9" xr3:uid="{1C111E93-F74B-4AF3-ACA9-F37B25591339}" name="Temporal Resolution" dataDxfId="16"/>
-    <tableColumn id="10" xr3:uid="{11DCA161-46A1-41D3-AE38-855C3E88B8D1}" name="Primary Uncertainty Source" dataDxfId="15"/>
-    <tableColumn id="11" xr3:uid="{39DAC786-D593-4CD5-B45E-91C6A12BB710}" name="Reliability Context" dataDxfId="14"/>
-    <tableColumn id="12" xr3:uid="{8A24A549-163F-412D-9F70-129B7376904B}" name="Typical Data Sources / Systems" dataDxfId="13"/>
+    <tableColumn id="13" xr3:uid="{8D7C28EE-960A-49A1-9FFC-CF5BAFA26C18}" name="Contributes To Question Types" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{AD6576F3-D2B1-477D-A460-9D7D8F000211}" name="Level1 Category" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{0C27C753-AF92-4769-9D92-64781AA12529}" name="Data Class" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{0347D29C-0658-4470-8597-C2BEB668EA32}" name="Observable Quantity" dataDxfId="17"/>
+    <tableColumn id="8" xr3:uid="{2418DCB6-00EA-4B5D-955A-FC9E0439D4FC}" name="Spatial Resolution" dataDxfId="16"/>
+    <tableColumn id="9" xr3:uid="{1C111E93-F74B-4AF3-ACA9-F37B25591339}" name="Temporal Resolution" dataDxfId="15"/>
+    <tableColumn id="10" xr3:uid="{11DCA161-46A1-41D3-AE38-855C3E88B8D1}" name="Primary Uncertainty Source" dataDxfId="14"/>
+    <tableColumn id="11" xr3:uid="{39DAC786-D593-4CD5-B45E-91C6A12BB710}" name="Reliability Context" dataDxfId="13"/>
+    <tableColumn id="12" xr3:uid="{8A24A549-163F-412D-9F70-129B7376904B}" name="Typical Data Sources / Systems" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{02922E52-8C1A-475B-BD8D-82F934F2E59F}" name="Table43" displayName="Table43" ref="A1:K112" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{02922E52-8C1A-475B-BD8D-82F934F2E59F}" name="Table43" displayName="Table43" ref="A1:K112" totalsRowShown="0" headerRowDxfId="11">
   <autoFilter ref="A1:K112" xr:uid="{02922E52-8C1A-475B-BD8D-82F934F2E59F}"/>
   <tableColumns count="11">
     <tableColumn id="2" xr3:uid="{D4418C6B-7D80-458E-A033-8C6DD9148AE1}" name="Level1 Category" dataDxfId="10"/>
@@ -2873,8 +3053,8 @@
     <tableColumn id="7" xr3:uid="{1B9BA010-3EE5-48F4-8C1F-4B0CBA5530DA}" name="Typical Max" dataDxfId="4"/>
     <tableColumn id="19" xr3:uid="{8511ED51-EB8C-4114-8709-1A5AB9C96E0B}" name="MF_Type" dataDxfId="3"/>
     <tableColumn id="20" xr3:uid="{04B31232-F121-42D2-9EFD-1C03E06913E0}" name="MF_Count" dataDxfId="2"/>
-    <tableColumn id="21" xr3:uid="{010F1FC7-105B-45F1-A4E7-04DB902D9AB9}" name="MF_Labels" dataDxfId="0"/>
-    <tableColumn id="22" xr3:uid="{699E24E4-08C1-4C8B-9C23-0CF54A3C5B67}" name="MF_Params" dataDxfId="1"/>
+    <tableColumn id="21" xr3:uid="{010F1FC7-105B-45F1-A4E7-04DB902D9AB9}" name="MF_Labels" dataDxfId="1"/>
+    <tableColumn id="22" xr3:uid="{699E24E4-08C1-4C8B-9C23-0CF54A3C5B67}" name="MF_Params" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7387,32 +7567,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51DF3B4E-BCAB-4AEC-B0D5-4F5824018DE1}">
   <dimension ref="A1:K112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C44" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K47" sqref="K47"/>
+    <sheetView tabSelected="1" topLeftCell="A104" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E108" sqref="E108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.140625" style="8" customWidth="1"/>
-    <col min="2" max="2" width="37.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.28515625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="27.140625" style="8" customWidth="1"/>
     <col min="4" max="4" width="37.140625" style="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.28515625" style="8" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" style="8" customWidth="1"/>
     <col min="7" max="7" width="9.42578125" style="8" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" style="8" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" style="8" customWidth="1"/>
     <col min="10" max="10" width="14.85546875" style="8" customWidth="1"/>
-    <col min="11" max="11" width="123.28515625" style="8" customWidth="1"/>
+    <col min="11" max="11" width="98.140625" style="8" customWidth="1"/>
     <col min="12" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>221</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>222</v>
@@ -7442,7 +7622,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>118</v>
       </c>
@@ -7453,7 +7633,7 @@
         <v>309</v>
       </c>
       <c r="D2" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="E2" t="s">
         <v>609</v>
@@ -7474,10 +7654,10 @@
         <v>674</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>824</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>118</v>
       </c>
@@ -7488,7 +7668,7 @@
         <v>231</v>
       </c>
       <c r="D3" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="E3" t="s">
         <v>609</v>
@@ -7509,10 +7689,10 @@
         <v>674</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>795</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>118</v>
       </c>
@@ -7523,7 +7703,7 @@
         <v>311</v>
       </c>
       <c r="D4" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="E4" t="s">
         <v>609</v>
@@ -7544,10 +7724,10 @@
         <v>674</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>796</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>118</v>
       </c>
@@ -7558,7 +7738,7 @@
         <v>313</v>
       </c>
       <c r="D5" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="E5" t="s">
         <v>609</v>
@@ -7579,10 +7759,10 @@
         <v>674</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>797</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>118</v>
       </c>
@@ -7593,7 +7773,7 @@
         <v>317</v>
       </c>
       <c r="D6" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="E6" t="s">
         <v>609</v>
@@ -7614,10 +7794,10 @@
         <v>674</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>798</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>118</v>
       </c>
@@ -7628,7 +7808,7 @@
         <v>322</v>
       </c>
       <c r="D7" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="E7" t="s">
         <v>609</v>
@@ -7649,10 +7829,10 @@
         <v>674</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>799</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>118</v>
       </c>
@@ -7663,7 +7843,7 @@
         <v>325</v>
       </c>
       <c r="D8" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="E8" t="s">
         <v>609</v>
@@ -7684,10 +7864,10 @@
         <v>674</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>118</v>
       </c>
@@ -7698,7 +7878,7 @@
         <v>330</v>
       </c>
       <c r="D9" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="E9" t="s">
         <v>609</v>
@@ -7719,10 +7899,10 @@
         <v>674</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>801</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>118</v>
       </c>
@@ -7733,7 +7913,7 @@
         <v>333</v>
       </c>
       <c r="D10" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="E10" t="s">
         <v>609</v>
@@ -7754,10 +7934,10 @@
         <v>674</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>802</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>118</v>
       </c>
@@ -7768,7 +7948,7 @@
         <v>334</v>
       </c>
       <c r="D11" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="E11" t="s">
         <v>609</v>
@@ -7789,10 +7969,10 @@
         <v>674</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>803</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>118</v>
       </c>
@@ -7803,7 +7983,7 @@
         <v>337</v>
       </c>
       <c r="D12" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="E12" t="s">
         <v>609</v>
@@ -7824,10 +8004,10 @@
         <v>674</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>835</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>118</v>
       </c>
@@ -7838,7 +8018,7 @@
         <v>340</v>
       </c>
       <c r="D13" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="E13" t="s">
         <v>609</v>
@@ -7859,7 +8039,7 @@
         <v>674</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>802</v>
+        <v>842</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -7873,7 +8053,7 @@
         <v>343</v>
       </c>
       <c r="D14" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="E14" t="s">
         <v>634</v>
@@ -7891,10 +8071,10 @@
         <v>5</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>834</v>
+        <v>821</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>836</v>
+        <v>822</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -7908,7 +8088,7 @@
         <v>347</v>
       </c>
       <c r="D15" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="E15" t="s">
         <v>610</v>
@@ -7929,10 +8109,10 @@
         <v>674</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>825</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>108</v>
       </c>
@@ -7943,7 +8123,7 @@
         <v>350</v>
       </c>
       <c r="D16" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="E16" t="s">
         <v>609</v>
@@ -7964,10 +8144,10 @@
         <v>674</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>835</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>108</v>
       </c>
@@ -7978,7 +8158,7 @@
         <v>351</v>
       </c>
       <c r="D17" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="E17" t="s">
         <v>610</v>
@@ -7999,10 +8179,10 @@
         <v>674</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>826</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>108</v>
       </c>
@@ -8013,7 +8193,7 @@
         <v>251</v>
       </c>
       <c r="D18" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="E18" t="s">
         <v>611</v>
@@ -8034,10 +8214,10 @@
         <v>674</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>807</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>108</v>
       </c>
@@ -8048,7 +8228,7 @@
         <v>353</v>
       </c>
       <c r="D19" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="E19" t="s">
         <v>609</v>
@@ -8069,10 +8249,10 @@
         <v>674</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>802</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>108</v>
       </c>
@@ -8083,7 +8263,7 @@
         <v>356</v>
       </c>
       <c r="D20" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="E20" t="s">
         <v>609</v>
@@ -8104,10 +8284,10 @@
         <v>674</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>802</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>108</v>
       </c>
@@ -8118,7 +8298,7 @@
         <v>360</v>
       </c>
       <c r="D21" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="E21" t="s">
         <v>609</v>
@@ -8139,10 +8319,10 @@
         <v>674</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>802</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>108</v>
       </c>
@@ -8153,7 +8333,7 @@
         <v>364</v>
       </c>
       <c r="D22" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="E22" t="s">
         <v>612</v>
@@ -8174,10 +8354,10 @@
         <v>674</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>827</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>108</v>
       </c>
@@ -8188,7 +8368,7 @@
         <v>368</v>
       </c>
       <c r="D23" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="E23" t="s">
         <v>613</v>
@@ -8209,10 +8389,10 @@
         <v>674</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>840</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>108</v>
       </c>
@@ -8223,7 +8403,7 @@
         <v>371</v>
       </c>
       <c r="D24" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="E24" t="s">
         <v>614</v>
@@ -8244,10 +8424,10 @@
         <v>674</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>828</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>138</v>
       </c>
@@ -8258,7 +8438,7 @@
         <v>254</v>
       </c>
       <c r="D25" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="E25" t="s">
         <v>615</v>
@@ -8279,10 +8459,10 @@
         <v>674</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>809</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>138</v>
       </c>
@@ -8293,7 +8473,7 @@
         <v>254</v>
       </c>
       <c r="D26" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="E26" t="s">
         <v>615</v>
@@ -8314,10 +8494,10 @@
         <v>674</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>810</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>138</v>
       </c>
@@ -8328,7 +8508,7 @@
         <v>374</v>
       </c>
       <c r="D27" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="E27" t="s">
         <v>609</v>
@@ -8349,10 +8529,10 @@
         <v>674</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>802</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>138</v>
       </c>
@@ -8363,7 +8543,7 @@
         <v>375</v>
       </c>
       <c r="D28" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="E28" t="s">
         <v>609</v>
@@ -8384,10 +8564,10 @@
         <v>674</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>802</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>138</v>
       </c>
@@ -8398,7 +8578,7 @@
         <v>262</v>
       </c>
       <c r="D29" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="E29" t="s">
         <v>609</v>
@@ -8419,10 +8599,10 @@
         <v>674</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>802</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>138</v>
       </c>
@@ -8433,7 +8613,7 @@
         <v>381</v>
       </c>
       <c r="D30" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="E30" t="s">
         <v>609</v>
@@ -8454,10 +8634,10 @@
         <v>674</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>802</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>138</v>
       </c>
@@ -8468,7 +8648,7 @@
         <v>384</v>
       </c>
       <c r="D31" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="E31" t="s">
         <v>610</v>
@@ -8489,7 +8669,7 @@
         <v>674</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>804</v>
+        <v>852</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -8503,7 +8683,7 @@
         <v>386</v>
       </c>
       <c r="D32" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="E32" t="s">
         <v>610</v>
@@ -8524,10 +8704,10 @@
         <v>674</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>811</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>138</v>
       </c>
@@ -8538,7 +8718,7 @@
         <v>388</v>
       </c>
       <c r="D33" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="E33" t="s">
         <v>609</v>
@@ -8559,10 +8739,10 @@
         <v>674</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>802</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>138</v>
       </c>
@@ -8573,7 +8753,7 @@
         <v>392</v>
       </c>
       <c r="D34" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="E34" t="s">
         <v>609</v>
@@ -8594,10 +8774,10 @@
         <v>674</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>802</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>147</v>
       </c>
@@ -8608,7 +8788,7 @@
         <v>396</v>
       </c>
       <c r="D35" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="E35" t="s">
         <v>610</v>
@@ -8629,10 +8809,10 @@
         <v>674</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>812</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>147</v>
       </c>
@@ -8643,7 +8823,7 @@
         <v>398</v>
       </c>
       <c r="D36" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="E36" t="s">
         <v>616</v>
@@ -8664,10 +8844,10 @@
         <v>674</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>804</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>147</v>
       </c>
@@ -8678,7 +8858,7 @@
         <v>399</v>
       </c>
       <c r="D37" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="E37" t="s">
         <v>616</v>
@@ -8690,19 +8870,19 @@
         <v>360</v>
       </c>
       <c r="H37" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="I37">
         <v>8</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>832</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>147</v>
       </c>
@@ -8713,7 +8893,7 @@
         <v>400</v>
       </c>
       <c r="D38" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="E38" t="s">
         <v>609</v>
@@ -8734,10 +8914,10 @@
         <v>674</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>802</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>147</v>
       </c>
@@ -8748,7 +8928,7 @@
         <v>271</v>
       </c>
       <c r="D39" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="E39" t="s">
         <v>609</v>
@@ -8769,10 +8949,10 @@
         <v>674</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>802</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>147</v>
       </c>
@@ -8783,7 +8963,7 @@
         <v>404</v>
       </c>
       <c r="D40" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="E40" t="s">
         <v>609</v>
@@ -8804,10 +8984,10 @@
         <v>674</v>
       </c>
       <c r="K40" s="2" t="s">
-        <v>802</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>147</v>
       </c>
@@ -8818,7 +8998,7 @@
         <v>407</v>
       </c>
       <c r="D41" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="E41" t="s">
         <v>609</v>
@@ -8839,10 +9019,10 @@
         <v>674</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>802</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>147</v>
       </c>
@@ -8853,7 +9033,7 @@
         <v>410</v>
       </c>
       <c r="D42" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="E42" t="s">
         <v>609</v>
@@ -8874,7 +9054,7 @@
         <v>674</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>802</v>
+        <v>860</v>
       </c>
     </row>
     <row r="43" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -8888,7 +9068,7 @@
         <v>157</v>
       </c>
       <c r="D43" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="E43" t="s">
         <v>273</v>
@@ -8909,10 +9089,10 @@
         <v>674</v>
       </c>
       <c r="K43" s="2" t="s">
-        <v>813</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>156</v>
       </c>
@@ -8923,7 +9103,7 @@
         <v>266</v>
       </c>
       <c r="D44" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="E44" t="s">
         <v>616</v>
@@ -8935,16 +9115,16 @@
         <v>360</v>
       </c>
       <c r="H44" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="I44">
         <v>8</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -8958,7 +9138,7 @@
         <v>412</v>
       </c>
       <c r="D45" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="E45" t="s">
         <v>273</v>
@@ -8982,7 +9162,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>156</v>
       </c>
@@ -8993,7 +9173,7 @@
         <v>415</v>
       </c>
       <c r="D46" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="E46" t="s">
         <v>273</v>
@@ -9014,7 +9194,7 @@
         <v>674</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>677</v>
+        <v>832</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -9028,7 +9208,7 @@
         <v>419</v>
       </c>
       <c r="D47" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="E47" t="s">
         <v>617</v>
@@ -9046,13 +9226,13 @@
         <v>5</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>841</v>
+        <v>825</v>
       </c>
       <c r="K47" s="2" t="s">
-        <v>844</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>156</v>
       </c>
@@ -9063,7 +9243,7 @@
         <v>421</v>
       </c>
       <c r="D48" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="E48" t="s">
         <v>610</v>
@@ -9084,10 +9264,10 @@
         <v>674</v>
       </c>
       <c r="K48" s="2" t="s">
-        <v>815</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>156</v>
       </c>
@@ -9098,7 +9278,7 @@
         <v>422</v>
       </c>
       <c r="D49" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="E49" t="s">
         <v>618</v>
@@ -9119,10 +9299,10 @@
         <v>674</v>
       </c>
       <c r="K49" s="2" t="s">
-        <v>829</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>156</v>
       </c>
@@ -9133,7 +9313,7 @@
         <v>423</v>
       </c>
       <c r="D50" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="E50" t="s">
         <v>615</v>
@@ -9154,10 +9334,10 @@
         <v>674</v>
       </c>
       <c r="K50" s="2" t="s">
-        <v>830</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>156</v>
       </c>
@@ -9168,7 +9348,7 @@
         <v>425</v>
       </c>
       <c r="D51" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="E51" t="s">
         <v>609</v>
@@ -9189,10 +9369,10 @@
         <v>674</v>
       </c>
       <c r="K51" s="2" t="s">
-        <v>835</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>156</v>
       </c>
@@ -9203,7 +9383,7 @@
         <v>428</v>
       </c>
       <c r="D52" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="E52" t="s">
         <v>609</v>
@@ -9224,10 +9404,10 @@
         <v>674</v>
       </c>
       <c r="K52" s="2" t="s">
-        <v>835</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>163</v>
       </c>
@@ -9235,10 +9415,10 @@
         <v>164</v>
       </c>
       <c r="C53" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="D53" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="E53" t="s">
         <v>280</v>
@@ -9259,10 +9439,10 @@
         <v>674</v>
       </c>
       <c r="K53" s="2" t="s">
-        <v>678</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>163</v>
       </c>
@@ -9273,7 +9453,7 @@
         <v>433</v>
       </c>
       <c r="D54" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="E54" t="s">
         <v>609</v>
@@ -9294,10 +9474,10 @@
         <v>674</v>
       </c>
       <c r="K54" s="2" t="s">
-        <v>835</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>163</v>
       </c>
@@ -9308,7 +9488,7 @@
         <v>437</v>
       </c>
       <c r="D55" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="E55" t="s">
         <v>619</v>
@@ -9329,10 +9509,10 @@
         <v>674</v>
       </c>
       <c r="K55" s="2" t="s">
-        <v>677</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>163</v>
       </c>
@@ -9343,7 +9523,7 @@
         <v>439</v>
       </c>
       <c r="D56" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="E56" t="s">
         <v>620</v>
@@ -9364,10 +9544,10 @@
         <v>674</v>
       </c>
       <c r="K56" s="2" t="s">
-        <v>817</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>163</v>
       </c>
@@ -9378,7 +9558,7 @@
         <v>442</v>
       </c>
       <c r="D57" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="E57" t="s">
         <v>609</v>
@@ -9399,10 +9579,10 @@
         <v>674</v>
       </c>
       <c r="K57" s="2" t="s">
-        <v>802</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>163</v>
       </c>
@@ -9413,7 +9593,7 @@
         <v>446</v>
       </c>
       <c r="D58" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="E58" t="s">
         <v>614</v>
@@ -9434,10 +9614,10 @@
         <v>674</v>
       </c>
       <c r="K58" s="2" t="s">
-        <v>807</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>163</v>
       </c>
@@ -9448,7 +9628,7 @@
         <v>449</v>
       </c>
       <c r="D59" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="E59" t="s">
         <v>614</v>
@@ -9469,7 +9649,7 @@
         <v>674</v>
       </c>
       <c r="K59" s="2" t="s">
-        <v>807</v>
+        <v>866</v>
       </c>
     </row>
     <row r="60" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -9483,7 +9663,7 @@
         <v>451</v>
       </c>
       <c r="D60" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="E60" t="s">
         <v>621</v>
@@ -9501,10 +9681,10 @@
         <v>5</v>
       </c>
       <c r="J60" s="2" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="K60" s="2" t="s">
-        <v>837</v>
+        <v>834</v>
       </c>
     </row>
     <row r="61" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -9518,7 +9698,7 @@
         <v>455</v>
       </c>
       <c r="D61" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="E61" t="s">
         <v>621</v>
@@ -9536,13 +9716,13 @@
         <v>5</v>
       </c>
       <c r="J61" s="2" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="K61" s="2" t="s">
-        <v>837</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>112</v>
       </c>
@@ -9553,7 +9733,7 @@
         <v>169</v>
       </c>
       <c r="D62" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="E62" t="s">
         <v>622</v>
@@ -9574,10 +9754,10 @@
         <v>674</v>
       </c>
       <c r="K62" s="2" t="s">
-        <v>818</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>112</v>
       </c>
@@ -9588,7 +9768,7 @@
         <v>460</v>
       </c>
       <c r="D63" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="E63" t="s">
         <v>609</v>
@@ -9609,7 +9789,7 @@
         <v>674</v>
       </c>
       <c r="K63" s="2" t="s">
-        <v>802</v>
+        <v>867</v>
       </c>
     </row>
     <row r="64" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -9623,7 +9803,7 @@
         <v>463</v>
       </c>
       <c r="D64" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="E64" t="s">
         <v>621</v>
@@ -9641,13 +9821,13 @@
         <v>5</v>
       </c>
       <c r="J64" s="2" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="K64" s="2" t="s">
-        <v>837</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>112</v>
       </c>
@@ -9658,7 +9838,7 @@
         <v>467</v>
       </c>
       <c r="D65" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="E65" t="s">
         <v>609</v>
@@ -9679,10 +9859,10 @@
         <v>674</v>
       </c>
       <c r="K65" s="2" t="s">
-        <v>802</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>112</v>
       </c>
@@ -9693,7 +9873,7 @@
         <v>469</v>
       </c>
       <c r="D66" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="E66" t="s">
         <v>609</v>
@@ -9714,10 +9894,10 @@
         <v>674</v>
       </c>
       <c r="K66" s="2" t="s">
-        <v>802</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>112</v>
       </c>
@@ -9728,7 +9908,7 @@
         <v>471</v>
       </c>
       <c r="D67" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E67" t="s">
         <v>609</v>
@@ -9749,10 +9929,10 @@
         <v>674</v>
       </c>
       <c r="K67" s="2" t="s">
-        <v>802</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>112</v>
       </c>
@@ -9763,7 +9943,7 @@
         <v>472</v>
       </c>
       <c r="D68" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E68" t="s">
         <v>609</v>
@@ -9784,10 +9964,10 @@
         <v>674</v>
       </c>
       <c r="K68" s="2" t="s">
-        <v>802</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>112</v>
       </c>
@@ -9798,7 +9978,7 @@
         <v>475</v>
       </c>
       <c r="D69" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="E69" t="s">
         <v>609</v>
@@ -9819,10 +9999,10 @@
         <v>674</v>
       </c>
       <c r="K69" s="2" t="s">
-        <v>802</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>112</v>
       </c>
@@ -9833,7 +10013,7 @@
         <v>479</v>
       </c>
       <c r="D70" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="E70" t="s">
         <v>609</v>
@@ -9854,10 +10034,10 @@
         <v>674</v>
       </c>
       <c r="K70" s="2" t="s">
-        <v>802</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>112</v>
       </c>
@@ -9868,7 +10048,7 @@
         <v>481</v>
       </c>
       <c r="D71" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="E71" t="s">
         <v>623</v>
@@ -9889,10 +10069,10 @@
         <v>674</v>
       </c>
       <c r="K71" s="2" t="s">
-        <v>808</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>112</v>
       </c>
@@ -9903,7 +10083,7 @@
         <v>485</v>
       </c>
       <c r="D72" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="E72" t="s">
         <v>609</v>
@@ -9924,7 +10104,7 @@
         <v>674</v>
       </c>
       <c r="K72" s="2" t="s">
-        <v>833</v>
+        <v>820</v>
       </c>
     </row>
     <row r="73" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -9938,7 +10118,7 @@
         <v>488</v>
       </c>
       <c r="D73" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="E73" t="s">
         <v>621</v>
@@ -9956,13 +10136,13 @@
         <v>5</v>
       </c>
       <c r="J73" s="2" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="K73" s="2" t="s">
-        <v>831</v>
-      </c>
-    </row>
-    <row r="74" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>175</v>
       </c>
@@ -9973,7 +10153,7 @@
         <v>491</v>
       </c>
       <c r="D74" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="E74" t="s">
         <v>612</v>
@@ -9994,7 +10174,7 @@
         <v>674</v>
       </c>
       <c r="K74" s="2" t="s">
-        <v>817</v>
+        <v>875</v>
       </c>
     </row>
     <row r="75" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -10008,7 +10188,7 @@
         <v>288</v>
       </c>
       <c r="D75" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="E75" t="s">
         <v>624</v>
@@ -10029,7 +10209,7 @@
         <v>674</v>
       </c>
       <c r="K75" s="2" t="s">
-        <v>819</v>
+        <v>876</v>
       </c>
     </row>
     <row r="76" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -10043,7 +10223,7 @@
         <v>496</v>
       </c>
       <c r="D76" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="E76" t="s">
         <v>625</v>
@@ -10061,13 +10241,13 @@
         <v>5</v>
       </c>
       <c r="J76" s="2" t="s">
-        <v>842</v>
+        <v>826</v>
       </c>
       <c r="K76" s="2" t="s">
-        <v>843</v>
-      </c>
-    </row>
-    <row r="77" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>175</v>
       </c>
@@ -10078,7 +10258,7 @@
         <v>500</v>
       </c>
       <c r="D77" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="E77" t="s">
         <v>612</v>
@@ -10099,10 +10279,10 @@
         <v>674</v>
       </c>
       <c r="K77" s="2" t="s">
-        <v>817</v>
-      </c>
-    </row>
-    <row r="78" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>175</v>
       </c>
@@ -10113,7 +10293,7 @@
         <v>502</v>
       </c>
       <c r="D78" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="E78" t="s">
         <v>626</v>
@@ -10134,10 +10314,10 @@
         <v>674</v>
       </c>
       <c r="K78" s="2" t="s">
-        <v>807</v>
-      </c>
-    </row>
-    <row r="79" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>175</v>
       </c>
@@ -10148,7 +10328,7 @@
         <v>505</v>
       </c>
       <c r="D79" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="E79" t="s">
         <v>627</v>
@@ -10169,10 +10349,10 @@
         <v>674</v>
       </c>
       <c r="K79" s="2" t="s">
-        <v>820</v>
-      </c>
-    </row>
-    <row r="80" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>175</v>
       </c>
@@ -10183,7 +10363,7 @@
         <v>507</v>
       </c>
       <c r="D80" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="E80" t="s">
         <v>609</v>
@@ -10204,10 +10384,10 @@
         <v>674</v>
       </c>
       <c r="K80" s="2" t="s">
-        <v>802</v>
-      </c>
-    </row>
-    <row r="81" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>175</v>
       </c>
@@ -10218,7 +10398,7 @@
         <v>179</v>
       </c>
       <c r="D81" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="E81" t="s">
         <v>612</v>
@@ -10239,10 +10419,10 @@
         <v>674</v>
       </c>
       <c r="K81" s="2" t="s">
-        <v>806</v>
-      </c>
-    </row>
-    <row r="82" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>175</v>
       </c>
@@ -10253,7 +10433,7 @@
         <v>510</v>
       </c>
       <c r="D82" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="E82" t="s">
         <v>612</v>
@@ -10274,10 +10454,10 @@
         <v>674</v>
       </c>
       <c r="K82" s="2" t="s">
-        <v>806</v>
-      </c>
-    </row>
-    <row r="83" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>175</v>
       </c>
@@ -10288,7 +10468,7 @@
         <v>512</v>
       </c>
       <c r="D83" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="E83" t="s">
         <v>609</v>
@@ -10309,10 +10489,10 @@
         <v>674</v>
       </c>
       <c r="K83" s="2" t="s">
-        <v>802</v>
-      </c>
-    </row>
-    <row r="84" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>181</v>
       </c>
@@ -10323,7 +10503,7 @@
         <v>515</v>
       </c>
       <c r="D84" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="E84" t="s">
         <v>612</v>
@@ -10344,10 +10524,10 @@
         <v>674</v>
       </c>
       <c r="K84" s="2" t="s">
-        <v>806</v>
-      </c>
-    </row>
-    <row r="85" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>181</v>
       </c>
@@ -10358,7 +10538,7 @@
         <v>183</v>
       </c>
       <c r="D85" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="E85" t="s">
         <v>626</v>
@@ -10379,10 +10559,10 @@
         <v>674</v>
       </c>
       <c r="K85" s="2" t="s">
-        <v>807</v>
-      </c>
-    </row>
-    <row r="86" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>181</v>
       </c>
@@ -10393,7 +10573,7 @@
         <v>515</v>
       </c>
       <c r="D86" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="E86" t="s">
         <v>612</v>
@@ -10414,10 +10594,10 @@
         <v>674</v>
       </c>
       <c r="K86" s="2" t="s">
-        <v>816</v>
-      </c>
-    </row>
-    <row r="87" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>181</v>
       </c>
@@ -10428,7 +10608,7 @@
         <v>185</v>
       </c>
       <c r="D87" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="E87" t="s">
         <v>626</v>
@@ -10449,10 +10629,10 @@
         <v>674</v>
       </c>
       <c r="K87" s="2" t="s">
-        <v>808</v>
-      </c>
-    </row>
-    <row r="88" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+        <v>886</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>181</v>
       </c>
@@ -10463,7 +10643,7 @@
         <v>521</v>
       </c>
       <c r="D88" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="E88" t="s">
         <v>626</v>
@@ -10484,7 +10664,7 @@
         <v>674</v>
       </c>
       <c r="K88" s="2" t="s">
-        <v>817</v>
+        <v>887</v>
       </c>
     </row>
     <row r="89" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -10498,7 +10678,7 @@
         <v>524</v>
       </c>
       <c r="D89" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="E89" t="s">
         <v>628</v>
@@ -10519,10 +10699,10 @@
         <v>674</v>
       </c>
       <c r="K89" s="2" t="s">
-        <v>814</v>
-      </c>
-    </row>
-    <row r="90" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>181</v>
       </c>
@@ -10533,7 +10713,7 @@
         <v>528</v>
       </c>
       <c r="D90" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="E90" t="s">
         <v>609</v>
@@ -10554,10 +10734,10 @@
         <v>674</v>
       </c>
       <c r="K90" s="2" t="s">
-        <v>802</v>
-      </c>
-    </row>
-    <row r="91" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>187</v>
       </c>
@@ -10568,7 +10748,7 @@
         <v>294</v>
       </c>
       <c r="D91" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="E91" t="s">
         <v>629</v>
@@ -10589,10 +10769,10 @@
         <v>674</v>
       </c>
       <c r="K91" s="2" t="s">
-        <v>821</v>
-      </c>
-    </row>
-    <row r="92" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+        <v>889</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>187</v>
       </c>
@@ -10603,7 +10783,7 @@
         <v>532</v>
       </c>
       <c r="D92" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="E92" t="s">
         <v>629</v>
@@ -10624,10 +10804,10 @@
         <v>674</v>
       </c>
       <c r="K92" s="2" t="s">
-        <v>821</v>
-      </c>
-    </row>
-    <row r="93" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>187</v>
       </c>
@@ -10638,7 +10818,7 @@
         <v>534</v>
       </c>
       <c r="D93" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="E93" t="s">
         <v>609</v>
@@ -10659,10 +10839,10 @@
         <v>674</v>
       </c>
       <c r="K93" s="2" t="s">
-        <v>802</v>
-      </c>
-    </row>
-    <row r="94" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>187</v>
       </c>
@@ -10673,7 +10853,7 @@
         <v>295</v>
       </c>
       <c r="D94" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="E94" t="s">
         <v>626</v>
@@ -10694,10 +10874,10 @@
         <v>674</v>
       </c>
       <c r="K94" s="2" t="s">
-        <v>822</v>
-      </c>
-    </row>
-    <row r="95" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>187</v>
       </c>
@@ -10708,7 +10888,7 @@
         <v>537</v>
       </c>
       <c r="D95" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="E95" t="s">
         <v>626</v>
@@ -10729,10 +10909,10 @@
         <v>674</v>
       </c>
       <c r="K95" s="2" t="s">
-        <v>821</v>
-      </c>
-    </row>
-    <row r="96" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>187</v>
       </c>
@@ -10743,7 +10923,7 @@
         <v>539</v>
       </c>
       <c r="D96" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="E96" t="s">
         <v>630</v>
@@ -10764,10 +10944,10 @@
         <v>674</v>
       </c>
       <c r="K96" s="2" t="s">
-        <v>823</v>
-      </c>
-    </row>
-    <row r="97" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>187</v>
       </c>
@@ -10778,7 +10958,7 @@
         <v>541</v>
       </c>
       <c r="D97" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="E97" t="s">
         <v>631</v>
@@ -10799,10 +10979,10 @@
         <v>674</v>
       </c>
       <c r="K97" s="2" t="s">
-        <v>820</v>
-      </c>
-    </row>
-    <row r="98" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>187</v>
       </c>
@@ -10813,7 +10993,7 @@
         <v>545</v>
       </c>
       <c r="D98" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="E98" t="s">
         <v>632</v>
@@ -10834,10 +11014,10 @@
         <v>674</v>
       </c>
       <c r="K98" s="2" t="s">
-        <v>805</v>
-      </c>
-    </row>
-    <row r="99" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>187</v>
       </c>
@@ -10848,7 +11028,7 @@
         <v>547</v>
       </c>
       <c r="D99" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="E99" t="s">
         <v>626</v>
@@ -10869,10 +11049,10 @@
         <v>674</v>
       </c>
       <c r="K99" s="2" t="s">
-        <v>821</v>
-      </c>
-    </row>
-    <row r="100" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>187</v>
       </c>
@@ -10883,7 +11063,7 @@
         <v>549</v>
       </c>
       <c r="D100" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="E100" t="s">
         <v>633</v>
@@ -10904,10 +11084,10 @@
         <v>674</v>
       </c>
       <c r="K100" s="2" t="s">
-        <v>817</v>
-      </c>
-    </row>
-    <row r="101" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>187</v>
       </c>
@@ -10918,7 +11098,7 @@
         <v>553</v>
       </c>
       <c r="D101" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="E101" t="s">
         <v>612</v>
@@ -10939,7 +11119,7 @@
         <v>674</v>
       </c>
       <c r="K101" s="2" t="s">
-        <v>805</v>
+        <v>897</v>
       </c>
     </row>
     <row r="102" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -10953,7 +11133,7 @@
         <v>556</v>
       </c>
       <c r="D102" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="E102" t="s">
         <v>621</v>
@@ -10971,13 +11151,13 @@
         <v>5</v>
       </c>
       <c r="J102" s="2" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="K102" s="2" t="s">
-        <v>831</v>
-      </c>
-    </row>
-    <row r="103" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>196</v>
       </c>
@@ -10988,7 +11168,7 @@
         <v>558</v>
       </c>
       <c r="D103" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="E103" t="s">
         <v>634</v>
@@ -11006,13 +11186,13 @@
         <v>5</v>
       </c>
       <c r="J103" s="2" t="s">
-        <v>834</v>
+        <v>821</v>
       </c>
       <c r="K103" s="2" t="s">
-        <v>838</v>
-      </c>
-    </row>
-    <row r="104" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>196</v>
       </c>
@@ -11023,7 +11203,7 @@
         <v>299</v>
       </c>
       <c r="D104" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="E104" t="s">
         <v>609</v>
@@ -11044,10 +11224,10 @@
         <v>674</v>
       </c>
       <c r="K104" s="2" t="s">
-        <v>802</v>
-      </c>
-    </row>
-    <row r="105" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>196</v>
       </c>
@@ -11058,7 +11238,7 @@
         <v>563</v>
       </c>
       <c r="D105" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="E105" t="s">
         <v>609</v>
@@ -11079,10 +11259,10 @@
         <v>674</v>
       </c>
       <c r="K105" s="2" t="s">
-        <v>835</v>
-      </c>
-    </row>
-    <row r="106" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>899</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>196</v>
       </c>
@@ -11093,7 +11273,7 @@
         <v>567</v>
       </c>
       <c r="D106" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="E106" t="s">
         <v>609</v>
@@ -11114,10 +11294,10 @@
         <v>674</v>
       </c>
       <c r="K106" s="2" t="s">
-        <v>802</v>
-      </c>
-    </row>
-    <row r="107" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>198</v>
       </c>
@@ -11128,7 +11308,7 @@
         <v>571</v>
       </c>
       <c r="D107" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="E107" t="s">
         <v>612</v>
@@ -11149,10 +11329,10 @@
         <v>674</v>
       </c>
       <c r="K107" s="2" t="s">
-        <v>820</v>
-      </c>
-    </row>
-    <row r="108" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>198</v>
       </c>
@@ -11163,7 +11343,7 @@
         <v>301</v>
       </c>
       <c r="D108" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="E108" t="s">
         <v>609</v>
@@ -11184,10 +11364,10 @@
         <v>674</v>
       </c>
       <c r="K108" s="2" t="s">
-        <v>802</v>
-      </c>
-    </row>
-    <row r="109" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>198</v>
       </c>
@@ -11198,7 +11378,7 @@
         <v>573</v>
       </c>
       <c r="D109" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="E109" t="s">
         <v>631</v>
@@ -11219,10 +11399,10 @@
         <v>674</v>
       </c>
       <c r="K109" s="2" t="s">
-        <v>808</v>
-      </c>
-    </row>
-    <row r="110" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>198</v>
       </c>
@@ -11233,7 +11413,7 @@
         <v>576</v>
       </c>
       <c r="D110" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="E110" t="s">
         <v>634</v>
@@ -11251,10 +11431,10 @@
         <v>5</v>
       </c>
       <c r="J110" s="2" t="s">
-        <v>834</v>
+        <v>821</v>
       </c>
       <c r="K110" s="2" t="s">
-        <v>839</v>
+        <v>824</v>
       </c>
     </row>
     <row r="111" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -11268,7 +11448,7 @@
         <v>580</v>
       </c>
       <c r="D111" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="E111" t="s">
         <v>624</v>
@@ -11289,10 +11469,10 @@
         <v>674</v>
       </c>
       <c r="K111" s="2" t="s">
-        <v>819</v>
-      </c>
-    </row>
-    <row r="112" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>198</v>
       </c>
@@ -11303,7 +11483,7 @@
         <v>582</v>
       </c>
       <c r="D112" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="E112" t="s">
         <v>612</v>
@@ -11324,7 +11504,7 @@
         <v>674</v>
       </c>
       <c r="K112" s="2" t="s">
-        <v>817</v>
+        <v>905</v>
       </c>
     </row>
   </sheetData>

</xml_diff>